<commit_message>
Fix missing optional in hashes, add analyze to jaen-convert
</commit_message>
<xml_diff>
--- a/schema_gen/openc2_genj.xlsx
+++ b/schema_gen/openc2_genj.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="756">
   <si>
-    <t>Generated from schema\openc2.jaen, Sat Apr  8 14:57:07 2017</t>
+    <t>Generated from schema\openc2.jaen, Tue Apr 11 09:47:03 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1056,7 +1056,7 @@
     <t>Hash values for algorithms included in hash-algo-ov</t>
   </si>
   <si>
-    <t>MD5 (required)</t>
+    <t>MD5 (optional)</t>
   </si>
   <si>
     <t>Hex (String)</t>
@@ -1065,79 +1065,79 @@
     <t>MD5 message digest as defined in RFC3121</t>
   </si>
   <si>
-    <t>MD6 (required)</t>
+    <t>MD6 (optional)</t>
   </si>
   <si>
     <t>MD6 message digest as defined in MD6 proposal</t>
   </si>
   <si>
-    <t>RIPEMD-160 (required)</t>
+    <t>RIPEMD-160 (optional)</t>
   </si>
   <si>
     <t>RACE Integrity Primitives Evaluation Message as defined in RIPEMD-160 specification</t>
   </si>
   <si>
-    <t>SHA-1 (required)</t>
+    <t>SHA-1 (optional)</t>
   </si>
   <si>
     <t>Secure Hash Algorithm (SHA)-1 as defined in RFC3174</t>
   </si>
   <si>
-    <t>SHA-224 (required)</t>
+    <t>SHA-224 (optional)</t>
   </si>
   <si>
     <t>SHA-224 as defined in RFC6234 (US Secure Hash Algorithms)</t>
   </si>
   <si>
-    <t>SHA-256 (required)</t>
+    <t>SHA-256 (optional)</t>
   </si>
   <si>
     <t>SHA-256 as defined in RFC6234</t>
   </si>
   <si>
-    <t>SHA-384 (required)</t>
+    <t>SHA-384 (optional)</t>
   </si>
   <si>
     <t>SHA-384 as defined in RFC6234</t>
   </si>
   <si>
-    <t>SHA-512 (required)</t>
+    <t>SHA-512 (optional)</t>
   </si>
   <si>
     <t>SHA-512 as defined in RFC6234</t>
   </si>
   <si>
-    <t>SHA3-224 (required)</t>
+    <t>SHA3-224 (optional)</t>
   </si>
   <si>
     <t>SHA3-224 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>SHA3-256 (required)</t>
+    <t>SHA3-256 (optional)</t>
   </si>
   <si>
     <t>SHA3-256 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>SHA3-384 (required)</t>
+    <t>SHA3-384 (optional)</t>
   </si>
   <si>
     <t>SHA3-384 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>SHA3-512 (required)</t>
+    <t>SHA3-512 (optional)</t>
   </si>
   <si>
     <t>SHA3-512 as defined in FIPS PUP 202</t>
   </si>
   <si>
-    <t>ssdeep (required)</t>
+    <t>ssdeep (optional)</t>
   </si>
   <si>
     <t>ssdeep fuzzy hashing algorithm as defined in the SSDEEP specification</t>
   </si>
   <si>
-    <t>WHIRLPOOL (required)</t>
+    <t>WHIRLPOOL (optional)</t>
   </si>
   <si>
     <t>whirlpool cryptographic hash function as defined in ISO/IEC 10118-3:2004</t>

</xml_diff>

<commit_message>
Add negotiation response, update JSON schema
</commit_message>
<xml_diff>
--- a/schema_gen/openc2_genj.xlsx
+++ b/schema_gen/openc2_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="758">
-  <si>
-    <t>Generated from schema\openc2.jaen, Thu May 11 16:10:34 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="797">
+  <si>
+    <t>Generated from schema\openc2.jaen, Tue May 23 12:30:11 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1338,6 +1338,12 @@
     <t>results = JAEN syntax of supported commands</t>
   </si>
   <si>
+    <t>communication</t>
+  </si>
+  <si>
+    <t>results = communication protocol parameters</t>
+  </si>
+  <si>
     <t>actuator_groups</t>
   </si>
   <si>
@@ -2290,6 +2296,117 @@
   </si>
   <si>
     <t>Specifies any hashes calculated for the entire contents of the certificate</t>
+  </si>
+  <si>
+    <t>comms</t>
+  </si>
+  <si>
+    <t>Structure that is returned in response to a "query communication" command</t>
+  </si>
+  <si>
+    <t>serialization (required)</t>
+  </si>
+  <si>
+    <t>serialization (vocab)</t>
+  </si>
+  <si>
+    <t>Payload serialization format</t>
+  </si>
+  <si>
+    <t>connection (required)</t>
+  </si>
+  <si>
+    <t>connection (Choice)</t>
+  </si>
+  <si>
+    <t>Connection protocol</t>
+  </si>
+  <si>
+    <t>serialization</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>JSON (uncompressed)</t>
+  </si>
+  <si>
+    <t>JSON-min</t>
+  </si>
+  <si>
+    <t>JSON Minified</t>
+  </si>
+  <si>
+    <t>CBOR</t>
+  </si>
+  <si>
+    <t>Concise Binary Object Representation (RFC 7049)</t>
+  </si>
+  <si>
+    <t>proto3</t>
+  </si>
+  <si>
+    <t>Google Protocol Buffers v3</t>
+  </si>
+  <si>
+    <t>XML</t>
+  </si>
+  <si>
+    <t>Extensible Markup Language</t>
+  </si>
+  <si>
+    <t>connection</t>
+  </si>
+  <si>
+    <t>REST</t>
+  </si>
+  <si>
+    <t>REST-params (Record)</t>
+  </si>
+  <si>
+    <t>Representational State Transfer web service protocol</t>
+  </si>
+  <si>
+    <t>DXL</t>
+  </si>
+  <si>
+    <t>DXL-params (Record)</t>
+  </si>
+  <si>
+    <t>Data Exchange Layer protocol</t>
+  </si>
+  <si>
+    <t>REST-params</t>
+  </si>
+  <si>
+    <t>port (required)</t>
+  </si>
+  <si>
+    <t>TCP/UDP port number or application protocol name</t>
+  </si>
+  <si>
+    <t>proto (required)</t>
+  </si>
+  <si>
+    <t>IP protocol (TCP, UDP, etc)</t>
+  </si>
+  <si>
+    <t>ipver (optional)</t>
+  </si>
+  <si>
+    <t>layer3-protocol (vocab)</t>
+  </si>
+  <si>
+    <t>IPv4 or v6</t>
+  </si>
+  <si>
+    <t>DXL-params</t>
+  </si>
+  <si>
+    <t>channel (required)</t>
+  </si>
+  <si>
+    <t>DXL channel name</t>
   </si>
 </sst>
 </file>
@@ -2773,7 +2890,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E631"/>
+  <dimension ref="A2:E665"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5382,7 +5499,7 @@
         <v>1</v>
       </c>
       <c r="C270" s="8" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D270" s="8" t="s">
         <v>43</v>
@@ -5394,7 +5511,7 @@
         <v>2</v>
       </c>
       <c r="C271" s="8" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D271" s="8" t="s">
         <v>43</v>
@@ -5406,7 +5523,7 @@
         <v>3</v>
       </c>
       <c r="C272" s="8" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D272" s="8" t="s">
         <v>43</v>
@@ -5418,7 +5535,7 @@
         <v>4</v>
       </c>
       <c r="C273" s="8" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D273" s="8" t="s">
         <v>43</v>
@@ -5430,7 +5547,7 @@
         <v>5</v>
       </c>
       <c r="C274" s="8" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D274" s="8" t="s">
         <v>43</v>
@@ -5442,7 +5559,7 @@
         <v>6</v>
       </c>
       <c r="C275" s="8" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D275" s="8" t="s">
         <v>43</v>
@@ -5454,7 +5571,7 @@
         <v>7</v>
       </c>
       <c r="C276" s="8" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D276" s="8" t="s">
         <v>43</v>
@@ -5502,13 +5619,13 @@
         <v>1</v>
       </c>
       <c r="C283" s="8" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D283" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E283" s="8" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -5516,13 +5633,13 @@
         <v>2</v>
       </c>
       <c r="C284" s="8" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D284" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E284" s="8" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="285" spans="1:5">
@@ -5530,13 +5647,13 @@
         <v>3</v>
       </c>
       <c r="C285" s="8" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D285" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -5544,13 +5661,13 @@
         <v>4</v>
       </c>
       <c r="C286" s="8" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D286" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="287" spans="1:5">
@@ -5558,13 +5675,13 @@
         <v>5</v>
       </c>
       <c r="C287" s="8" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D287" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E287" s="8" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="288" spans="1:5">
@@ -5572,13 +5689,13 @@
         <v>6</v>
       </c>
       <c r="C288" s="8" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D288" s="8" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E288" s="8" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="291" spans="1:5">
@@ -5586,7 +5703,7 @@
         <v>15</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C291" s="5"/>
       <c r="D291" s="5"/>
@@ -5597,7 +5714,7 @@
         <v>16</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C292" s="6"/>
       <c r="D292" s="6"/>
@@ -5609,7 +5726,7 @@
       </c>
       <c r="C293" s="8"/>
       <c r="D293" s="8" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E293" s="8"/>
     </row>
@@ -5618,7 +5735,7 @@
         <v>15</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C296" s="5"/>
       <c r="D296" s="5"/>
@@ -5654,7 +5771,7 @@
         <v>1</v>
       </c>
       <c r="C300" s="8" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D300" s="8" t="s">
         <v>137</v>
@@ -5666,7 +5783,7 @@
         <v>2</v>
       </c>
       <c r="C301" s="8" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D301" s="8" t="s">
         <v>149</v>
@@ -5725,7 +5842,7 @@
         <v>15</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C311" s="5"/>
       <c r="D311" s="5"/>
@@ -5772,7 +5889,7 @@
         <v>15</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C318" s="5"/>
       <c r="D318" s="5"/>
@@ -5808,13 +5925,13 @@
         <v>1</v>
       </c>
       <c r="C322" s="8" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D322" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E322" s="8" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="323" spans="1:5">
@@ -5822,13 +5939,13 @@
         <v>2</v>
       </c>
       <c r="C323" s="8" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D323" s="8" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="E323" s="8" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="326" spans="1:5">
@@ -5836,7 +5953,7 @@
         <v>15</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C326" s="5"/>
       <c r="D326" s="5"/>
@@ -5847,7 +5964,7 @@
         <v>16</v>
       </c>
       <c r="B327" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C327" s="6"/>
       <c r="D327" s="6"/>
@@ -5859,7 +5976,7 @@
       </c>
       <c r="C328" s="8"/>
       <c r="D328" s="8" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E328" s="8"/>
     </row>
@@ -5868,7 +5985,7 @@
         <v>15</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C331" s="5"/>
       <c r="D331" s="5"/>
@@ -5904,7 +6021,7 @@
         <v>1</v>
       </c>
       <c r="C335" s="8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D335" s="8" t="s">
         <v>151</v>
@@ -5916,7 +6033,7 @@
         <v>2</v>
       </c>
       <c r="C336" s="8" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D336" s="8" t="s">
         <v>153</v>
@@ -5928,7 +6045,7 @@
         <v>3</v>
       </c>
       <c r="C337" s="8" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D337" s="8" t="s">
         <v>143</v>
@@ -5940,7 +6057,7 @@
         <v>15</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C340" s="5"/>
       <c r="D340" s="5"/>
@@ -5976,13 +6093,13 @@
         <v>1</v>
       </c>
       <c r="C344" s="8" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D344" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E344" s="8" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="345" spans="1:5">
@@ -5990,13 +6107,13 @@
         <v>2</v>
       </c>
       <c r="C345" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D345" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E345" s="8" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="346" spans="1:5">
@@ -6004,13 +6121,13 @@
         <v>3</v>
       </c>
       <c r="C346" s="8" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D346" s="8" t="s">
         <v>168</v>
       </c>
       <c r="E346" s="8" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="349" spans="1:5">
@@ -6018,7 +6135,7 @@
         <v>15</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C349" s="5"/>
       <c r="D349" s="5"/>
@@ -6040,7 +6157,7 @@
         <v>125</v>
       </c>
       <c r="B351" s="6" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C351" s="6"/>
       <c r="D351" s="6"/>
@@ -6101,13 +6218,13 @@
         <v>1</v>
       </c>
       <c r="C360" s="8" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D360" s="8" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E360" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="361" spans="1:5">
@@ -6121,7 +6238,7 @@
         <v>420</v>
       </c>
       <c r="E361" s="8" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="362" spans="1:5">
@@ -6129,13 +6246,13 @@
         <v>3</v>
       </c>
       <c r="C362" s="8" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D362" s="8" t="s">
         <v>429</v>
       </c>
       <c r="E362" s="8" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="363" spans="1:5">
@@ -6149,7 +6266,7 @@
         <v>43</v>
       </c>
       <c r="E363" s="8" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="364" spans="1:5">
@@ -6157,13 +6274,13 @@
         <v>5</v>
       </c>
       <c r="C364" s="8" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D364" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="365" spans="1:5">
@@ -6171,13 +6288,13 @@
         <v>6</v>
       </c>
       <c r="C365" s="8" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D365" s="8" t="s">
         <v>346</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="366" spans="1:5">
@@ -6191,7 +6308,7 @@
         <v>43</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="367" spans="1:5">
@@ -6199,13 +6316,13 @@
         <v>8</v>
       </c>
       <c r="C367" s="8" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D367" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E367" s="8" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="368" spans="1:5">
@@ -6213,13 +6330,13 @@
         <v>9</v>
       </c>
       <c r="C368" s="8" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D368" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="369" spans="1:5">
@@ -6227,13 +6344,13 @@
         <v>10</v>
       </c>
       <c r="C369" s="8" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D369" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="370" spans="1:5">
@@ -6241,13 +6358,13 @@
         <v>11</v>
       </c>
       <c r="C370" s="8" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D370" s="8" t="s">
         <v>137</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="371" spans="1:5">
@@ -6255,13 +6372,13 @@
         <v>12</v>
       </c>
       <c r="C371" s="8" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D371" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E371" s="8" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="372" spans="1:5">
@@ -6269,13 +6386,13 @@
         <v>13</v>
       </c>
       <c r="C372" s="8" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D372" s="8" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="373" spans="1:5">
@@ -6283,13 +6400,13 @@
         <v>14</v>
       </c>
       <c r="C373" s="8" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="D373" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E373" s="8" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="374" spans="1:5">
@@ -6297,13 +6414,13 @@
         <v>15</v>
       </c>
       <c r="C374" s="8" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D374" s="8" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="375" spans="1:5">
@@ -6311,13 +6428,13 @@
         <v>16</v>
       </c>
       <c r="C375" s="8" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D375" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="378" spans="1:5">
@@ -6325,7 +6442,7 @@
         <v>15</v>
       </c>
       <c r="B378" s="5" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C378" s="5"/>
       <c r="D378" s="5"/>
@@ -6336,7 +6453,7 @@
         <v>16</v>
       </c>
       <c r="B379" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C379" s="6"/>
       <c r="D379" s="6"/>
@@ -6357,7 +6474,7 @@
         <v>15</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C383" s="5"/>
       <c r="D383" s="5"/>
@@ -6393,10 +6510,10 @@
         <v>1</v>
       </c>
       <c r="C387" s="8" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D387" s="8" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E387" s="8"/>
     </row>
@@ -6405,10 +6522,10 @@
         <v>2</v>
       </c>
       <c r="C388" s="8" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D388" s="8" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E388" s="8"/>
     </row>
@@ -6417,10 +6534,10 @@
         <v>3</v>
       </c>
       <c r="C389" s="8" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D389" s="8" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E389" s="8"/>
     </row>
@@ -6429,10 +6546,10 @@
         <v>4</v>
       </c>
       <c r="C390" s="8" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D390" s="8" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E390" s="8"/>
     </row>
@@ -6441,10 +6558,10 @@
         <v>5</v>
       </c>
       <c r="C391" s="8" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D391" s="8" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E391" s="8"/>
     </row>
@@ -6453,7 +6570,7 @@
         <v>15</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C394" s="5"/>
       <c r="D394" s="5"/>
@@ -6475,7 +6592,7 @@
         <v>125</v>
       </c>
       <c r="B396" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C396" s="6"/>
       <c r="D396" s="6"/>
@@ -6500,7 +6617,7 @@
         <v>15</v>
       </c>
       <c r="B401" s="5" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C401" s="5"/>
       <c r="D401" s="5"/>
@@ -6522,7 +6639,7 @@
         <v>125</v>
       </c>
       <c r="B403" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C403" s="6"/>
       <c r="D403" s="6"/>
@@ -6547,7 +6664,7 @@
         <v>15</v>
       </c>
       <c r="B408" s="5" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C408" s="5"/>
       <c r="D408" s="5"/>
@@ -6569,7 +6686,7 @@
         <v>125</v>
       </c>
       <c r="B410" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C410" s="6"/>
       <c r="D410" s="6"/>
@@ -6594,7 +6711,7 @@
         <v>15</v>
       </c>
       <c r="B415" s="5" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C415" s="5"/>
       <c r="D415" s="5"/>
@@ -6616,7 +6733,7 @@
         <v>125</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C417" s="6"/>
       <c r="D417" s="6"/>
@@ -6641,7 +6758,7 @@
         <v>15</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C422" s="5"/>
       <c r="D422" s="5"/>
@@ -6663,7 +6780,7 @@
         <v>125</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C424" s="6"/>
       <c r="D424" s="6"/>
@@ -6688,7 +6805,7 @@
         <v>15</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C429" s="5"/>
       <c r="D429" s="5"/>
@@ -6724,13 +6841,13 @@
         <v>1</v>
       </c>
       <c r="C433" s="8" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D433" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E433" s="8" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="434" spans="1:5">
@@ -6738,13 +6855,13 @@
         <v>2</v>
       </c>
       <c r="C434" s="8" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="D434" s="8" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E434" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="435" spans="1:5">
@@ -6752,13 +6869,13 @@
         <v>3</v>
       </c>
       <c r="C435" s="8" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D435" s="8" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E435" s="8" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="438" spans="1:5">
@@ -6766,7 +6883,7 @@
         <v>15</v>
       </c>
       <c r="B438" s="5" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C438" s="5"/>
       <c r="D438" s="5"/>
@@ -6802,13 +6919,13 @@
         <v>1</v>
       </c>
       <c r="C442" s="8" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D442" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E442" s="8" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="443" spans="1:5">
@@ -6816,13 +6933,13 @@
         <v>2</v>
       </c>
       <c r="C443" s="8" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="D443" s="8" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E443" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="444" spans="1:5">
@@ -6830,13 +6947,13 @@
         <v>3</v>
       </c>
       <c r="C444" s="8" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D444" s="8" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E444" s="8" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="447" spans="1:5">
@@ -6844,7 +6961,7 @@
         <v>15</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C447" s="5"/>
       <c r="D447" s="5"/>
@@ -6855,7 +6972,7 @@
         <v>16</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C448" s="6"/>
       <c r="D448" s="6"/>
@@ -6876,7 +6993,7 @@
         <v>15</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C452" s="5"/>
       <c r="D452" s="5"/>
@@ -6898,7 +7015,7 @@
         <v>125</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C454" s="6"/>
       <c r="D454" s="6"/>
@@ -6909,7 +7026,7 @@
         <v>15</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C457" s="5"/>
       <c r="D457" s="5"/>
@@ -6920,7 +7037,7 @@
         <v>16</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C458" s="6"/>
       <c r="D458" s="6"/>
@@ -6932,7 +7049,7 @@
       </c>
       <c r="C459" s="8"/>
       <c r="D459" s="8" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E459" s="8"/>
     </row>
@@ -6941,7 +7058,7 @@
         <v>15</v>
       </c>
       <c r="B462" s="5" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C462" s="5"/>
       <c r="D462" s="5"/>
@@ -6963,7 +7080,7 @@
         <v>125</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C464" s="6"/>
       <c r="D464" s="6"/>
@@ -6988,13 +7105,13 @@
         <v>1</v>
       </c>
       <c r="C467" s="8" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D467" s="8" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E467" s="8" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="468" spans="1:5">
@@ -7002,13 +7119,13 @@
         <v>2</v>
       </c>
       <c r="C468" s="8" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D468" s="8" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="E468" s="8" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="469" spans="1:5">
@@ -7016,13 +7133,13 @@
         <v>3</v>
       </c>
       <c r="C469" s="8" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D469" s="8" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E469" s="8" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="470" spans="1:5">
@@ -7030,13 +7147,13 @@
         <v>4</v>
       </c>
       <c r="C470" s="8" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D470" s="8" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="E470" s="8" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="471" spans="1:5">
@@ -7044,13 +7161,13 @@
         <v>5</v>
       </c>
       <c r="C471" s="8" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D471" s="8" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E471" s="8" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="474" spans="1:5">
@@ -7058,7 +7175,7 @@
         <v>15</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C474" s="5"/>
       <c r="D474" s="5"/>
@@ -7080,7 +7197,7 @@
         <v>125</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C476" s="6"/>
       <c r="D476" s="6"/>
@@ -7105,13 +7222,13 @@
         <v>1</v>
       </c>
       <c r="C479" s="8" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D479" s="8" t="s">
         <v>429</v>
       </c>
       <c r="E479" s="8" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="480" spans="1:5">
@@ -7119,13 +7236,13 @@
         <v>2</v>
       </c>
       <c r="C480" s="8" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D480" s="8" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="E480" s="8" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="483" spans="1:5">
@@ -7216,13 +7333,13 @@
         <v>1</v>
       </c>
       <c r="C494" s="8" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D494" s="8" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="E494" s="8" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="495" spans="1:5">
@@ -7230,13 +7347,13 @@
         <v>2</v>
       </c>
       <c r="C495" s="8" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D495" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E495" s="8" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="496" spans="1:5">
@@ -7244,13 +7361,13 @@
         <v>3</v>
       </c>
       <c r="C496" s="8" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D496" s="8" t="s">
         <v>429</v>
       </c>
       <c r="E496" s="8" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="497" spans="1:5">
@@ -7264,7 +7381,7 @@
         <v>43</v>
       </c>
       <c r="E497" s="8" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="498" spans="1:5">
@@ -7272,13 +7389,13 @@
         <v>5</v>
       </c>
       <c r="C498" s="8" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D498" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E498" s="8" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="499" spans="1:5">
@@ -7286,13 +7403,13 @@
         <v>6</v>
       </c>
       <c r="C499" s="8" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D499" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E499" s="8" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="500" spans="1:5">
@@ -7300,13 +7417,13 @@
         <v>7</v>
       </c>
       <c r="C500" s="8" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D500" s="8" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="E500" s="8" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="501" spans="1:5">
@@ -7314,13 +7431,13 @@
         <v>8</v>
       </c>
       <c r="C501" s="8" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="D501" s="8" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="E501" s="8" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="502" spans="1:5">
@@ -7328,13 +7445,13 @@
         <v>9</v>
       </c>
       <c r="C502" s="8" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="D502" s="8" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="E502" s="8" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="503" spans="1:5">
@@ -7342,13 +7459,13 @@
         <v>10</v>
       </c>
       <c r="C503" s="8" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D503" s="8" t="s">
         <v>168</v>
       </c>
       <c r="E503" s="8" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="504" spans="1:5">
@@ -7356,13 +7473,13 @@
         <v>11</v>
       </c>
       <c r="C504" s="8" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D504" s="8" t="s">
         <v>149</v>
       </c>
       <c r="E504" s="8" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="505" spans="1:5">
@@ -7370,13 +7487,13 @@
         <v>12</v>
       </c>
       <c r="C505" s="8" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D505" s="8" t="s">
         <v>162</v>
       </c>
       <c r="E505" s="8" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="506" spans="1:5">
@@ -7384,13 +7501,13 @@
         <v>13</v>
       </c>
       <c r="C506" s="8" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D506" s="8" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="E506" s="8" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="509" spans="1:5">
@@ -7398,7 +7515,7 @@
         <v>15</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C509" s="5"/>
       <c r="D509" s="5"/>
@@ -7409,7 +7526,7 @@
         <v>16</v>
       </c>
       <c r="B510" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C510" s="6"/>
       <c r="D510" s="6"/>
@@ -7430,7 +7547,7 @@
         <v>15</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="C514" s="5"/>
       <c r="D514" s="5"/>
@@ -7441,7 +7558,7 @@
         <v>16</v>
       </c>
       <c r="B515" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C515" s="6"/>
       <c r="D515" s="6"/>
@@ -7462,7 +7579,7 @@
         <v>15</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="C519" s="5"/>
       <c r="D519" s="5"/>
@@ -7473,7 +7590,7 @@
         <v>16</v>
       </c>
       <c r="B520" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C520" s="6"/>
       <c r="D520" s="6"/>
@@ -7494,7 +7611,7 @@
         <v>15</v>
       </c>
       <c r="B524" s="5" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C524" s="5"/>
       <c r="D524" s="5"/>
@@ -7530,10 +7647,10 @@
         <v>1</v>
       </c>
       <c r="C528" s="8" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D528" s="8" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E528" s="8"/>
     </row>
@@ -7542,10 +7659,10 @@
         <v>2</v>
       </c>
       <c r="C529" s="8" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="D529" s="8" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E529" s="8"/>
     </row>
@@ -7554,7 +7671,7 @@
         <v>15</v>
       </c>
       <c r="B532" s="5" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C532" s="5"/>
       <c r="D532" s="5"/>
@@ -7565,7 +7682,7 @@
         <v>16</v>
       </c>
       <c r="B533" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C533" s="6"/>
       <c r="D533" s="6"/>
@@ -7586,7 +7703,7 @@
         <v>15</v>
       </c>
       <c r="B537" s="5" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="C537" s="5"/>
       <c r="D537" s="5"/>
@@ -7608,7 +7725,7 @@
         <v>125</v>
       </c>
       <c r="B539" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C539" s="6"/>
       <c r="D539" s="6"/>
@@ -7633,7 +7750,7 @@
         <v>15</v>
       </c>
       <c r="B544" s="5" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C544" s="5"/>
       <c r="D544" s="5"/>
@@ -7655,7 +7772,7 @@
         <v>125</v>
       </c>
       <c r="B546" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C546" s="6"/>
       <c r="D546" s="6"/>
@@ -7716,13 +7833,13 @@
         <v>1</v>
       </c>
       <c r="C555" s="8" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D555" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E555" s="8" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="556" spans="1:5">
@@ -7730,13 +7847,13 @@
         <v>2</v>
       </c>
       <c r="C556" s="8" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D556" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E556" s="8" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="557" spans="1:5">
@@ -7744,13 +7861,13 @@
         <v>3</v>
       </c>
       <c r="C557" s="8" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="D557" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E557" s="8" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="558" spans="1:5">
@@ -7758,13 +7875,13 @@
         <v>4</v>
       </c>
       <c r="C558" s="8" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D558" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E558" s="8" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="559" spans="1:5">
@@ -7772,13 +7889,13 @@
         <v>5</v>
       </c>
       <c r="C559" s="8" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="D559" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E559" s="8" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="562" spans="1:5">
@@ -7808,7 +7925,7 @@
         <v>125</v>
       </c>
       <c r="B564" s="6" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C564" s="6"/>
       <c r="D564" s="6"/>
@@ -7819,7 +7936,7 @@
         <v>15</v>
       </c>
       <c r="B567" s="5" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="C567" s="5"/>
       <c r="D567" s="5"/>
@@ -7855,13 +7972,13 @@
         <v>1</v>
       </c>
       <c r="C571" s="8" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D571" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E571" s="8" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="572" spans="1:5">
@@ -7869,13 +7986,13 @@
         <v>2</v>
       </c>
       <c r="C572" s="8" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D572" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E572" s="8" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="573" spans="1:5">
@@ -7883,13 +8000,13 @@
         <v>3</v>
       </c>
       <c r="C573" s="8" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D573" s="8" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="E573" s="8" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="574" spans="1:5">
@@ -7897,13 +8014,13 @@
         <v>4</v>
       </c>
       <c r="C574" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D574" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E574" s="8" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="575" spans="1:5">
@@ -7911,13 +8028,13 @@
         <v>5</v>
       </c>
       <c r="C575" s="8" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D575" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E575" s="8" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="576" spans="1:5">
@@ -7925,13 +8042,13 @@
         <v>6</v>
       </c>
       <c r="C576" s="8" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="D576" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E576" s="8" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="577" spans="1:5">
@@ -7939,13 +8056,13 @@
         <v>7</v>
       </c>
       <c r="C577" s="8" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="D577" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E577" s="8" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="578" spans="1:5">
@@ -7953,13 +8070,13 @@
         <v>8</v>
       </c>
       <c r="C578" s="8" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D578" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E578" s="8" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="579" spans="1:5">
@@ -7967,13 +8084,13 @@
         <v>9</v>
       </c>
       <c r="C579" s="8" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="D579" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E579" s="8" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="580" spans="1:5">
@@ -7981,13 +8098,13 @@
         <v>10</v>
       </c>
       <c r="C580" s="8" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="D580" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E580" s="8" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="581" spans="1:5">
@@ -7995,13 +8112,13 @@
         <v>11</v>
       </c>
       <c r="C581" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D581" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E581" s="8" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="582" spans="1:5">
@@ -8009,13 +8126,13 @@
         <v>12</v>
       </c>
       <c r="C582" s="8" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D582" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E582" s="8" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="583" spans="1:5">
@@ -8023,13 +8140,13 @@
         <v>13</v>
       </c>
       <c r="C583" s="8" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="D583" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E583" s="8" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="586" spans="1:5">
@@ -8037,7 +8154,7 @@
         <v>15</v>
       </c>
       <c r="B586" s="5" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C586" s="5"/>
       <c r="D586" s="5"/>
@@ -8131,7 +8248,7 @@
         <v>15</v>
       </c>
       <c r="B600" s="5" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C600" s="5"/>
       <c r="D600" s="5"/>
@@ -8167,13 +8284,13 @@
         <v>1</v>
       </c>
       <c r="C604" s="8" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D604" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E604" s="8" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
     </row>
     <row r="605" spans="1:5">
@@ -8181,13 +8298,13 @@
         <v>2</v>
       </c>
       <c r="C605" s="8" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="D605" s="8" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="E605" s="8" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="606" spans="1:5">
@@ -8195,13 +8312,13 @@
         <v>3</v>
       </c>
       <c r="C606" s="8" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D606" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E606" s="8" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="607" spans="1:5">
@@ -8209,13 +8326,13 @@
         <v>4</v>
       </c>
       <c r="C607" s="8" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D607" s="8" t="s">
         <v>168</v>
       </c>
       <c r="E607" s="8" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="608" spans="1:5">
@@ -8223,13 +8340,13 @@
         <v>5</v>
       </c>
       <c r="C608" s="8" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="D608" s="8" t="s">
         <v>429</v>
       </c>
       <c r="E608" s="8" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
     </row>
     <row r="611" spans="1:5">
@@ -8237,7 +8354,7 @@
         <v>15</v>
       </c>
       <c r="B611" s="5" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C611" s="5"/>
       <c r="D611" s="5"/>
@@ -8248,7 +8365,7 @@
         <v>16</v>
       </c>
       <c r="B612" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C612" s="6"/>
       <c r="D612" s="6"/>
@@ -8260,7 +8377,7 @@
       </c>
       <c r="C613" s="8"/>
       <c r="D613" s="8" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="E613" s="8"/>
     </row>
@@ -8269,7 +8386,7 @@
         <v>15</v>
       </c>
       <c r="B616" s="5" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C616" s="5"/>
       <c r="D616" s="5"/>
@@ -8305,13 +8422,13 @@
         <v>1</v>
       </c>
       <c r="C620" s="8" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D620" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E620" s="8" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="621" spans="1:5">
@@ -8319,13 +8436,13 @@
         <v>2</v>
       </c>
       <c r="C621" s="8" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D621" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E621" s="8" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
     </row>
     <row r="622" spans="1:5">
@@ -8333,13 +8450,13 @@
         <v>3</v>
       </c>
       <c r="C622" s="8" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="D622" s="8" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="E622" s="8" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="625" spans="1:5">
@@ -8347,7 +8464,7 @@
         <v>15</v>
       </c>
       <c r="B625" s="5" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C625" s="5"/>
       <c r="D625" s="5"/>
@@ -8369,7 +8486,7 @@
         <v>125</v>
       </c>
       <c r="B627" s="6" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C627" s="6"/>
       <c r="D627" s="6"/>
@@ -8394,13 +8511,13 @@
         <v>1</v>
       </c>
       <c r="C630" s="8" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="D630" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E630" s="8" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="631" spans="1:5">
@@ -8408,17 +8525,295 @@
         <v>2</v>
       </c>
       <c r="C631" s="8" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="D631" s="8" t="s">
         <v>420</v>
       </c>
       <c r="E631" s="8" t="s">
-        <v>757</v>
+        <v>759</v>
+      </c>
+    </row>
+    <row r="634" spans="1:5">
+      <c r="A634" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B634" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="C634" s="5"/>
+      <c r="D634" s="5"/>
+      <c r="E634" s="5"/>
+    </row>
+    <row r="635" spans="1:5">
+      <c r="A635" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B635" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C635" s="6"/>
+      <c r="D635" s="6"/>
+      <c r="E635" s="6"/>
+    </row>
+    <row r="636" spans="1:5">
+      <c r="A636" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B636" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="C636" s="6"/>
+      <c r="D636" s="6"/>
+      <c r="E636" s="6"/>
+    </row>
+    <row r="638" spans="1:5">
+      <c r="B638" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C638" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D638" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E638" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="639" spans="1:5">
+      <c r="B639" s="8">
+        <v>1</v>
+      </c>
+      <c r="C639" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="D639" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="E639" s="8" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="640" spans="1:5">
+      <c r="B640" s="8">
+        <v>2</v>
+      </c>
+      <c r="C640" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="D640" s="8" t="s">
+        <v>766</v>
+      </c>
+      <c r="E640" s="8" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="643" spans="1:5">
+      <c r="A643" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B643" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="C643" s="5"/>
+      <c r="D643" s="5"/>
+      <c r="E643" s="5"/>
+    </row>
+    <row r="644" spans="1:5">
+      <c r="A644" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B644" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C644" s="6"/>
+      <c r="D644" s="6"/>
+      <c r="E644" s="6"/>
+    </row>
+    <row r="645" spans="1:5">
+      <c r="A645" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B645" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="C645" s="6"/>
+      <c r="D645" s="6"/>
+      <c r="E645" s="6"/>
+    </row>
+    <row r="647" spans="1:5">
+      <c r="B647" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C647" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D647" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E647" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="648" spans="1:5">
+      <c r="B648" s="8">
+        <v>1</v>
+      </c>
+      <c r="C648" s="8" t="s">
+        <v>780</v>
+      </c>
+      <c r="D648" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="E648" s="8" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="649" spans="1:5">
+      <c r="B649" s="8">
+        <v>2</v>
+      </c>
+      <c r="C649" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="D649" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="E649" s="8" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="652" spans="1:5">
+      <c r="A652" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B652" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="C652" s="5"/>
+      <c r="D652" s="5"/>
+      <c r="E652" s="5"/>
+    </row>
+    <row r="653" spans="1:5">
+      <c r="A653" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B653" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C653" s="6"/>
+      <c r="D653" s="6"/>
+      <c r="E653" s="6"/>
+    </row>
+    <row r="655" spans="1:5">
+      <c r="B655" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C655" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D655" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E655" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="656" spans="1:5">
+      <c r="B656" s="8">
+        <v>1</v>
+      </c>
+      <c r="C656" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="D656" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="E656" s="8" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="657" spans="1:5">
+      <c r="B657" s="8">
+        <v>2</v>
+      </c>
+      <c r="C657" s="8" t="s">
+        <v>789</v>
+      </c>
+      <c r="D657" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="E657" s="8" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="658" spans="1:5">
+      <c r="B658" s="8">
+        <v>3</v>
+      </c>
+      <c r="C658" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="D658" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="E658" s="8" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="661" spans="1:5">
+      <c r="A661" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B661" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="C661" s="5"/>
+      <c r="D661" s="5"/>
+      <c r="E661" s="5"/>
+    </row>
+    <row r="662" spans="1:5">
+      <c r="A662" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B662" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C662" s="6"/>
+      <c r="D662" s="6"/>
+      <c r="E662" s="6"/>
+    </row>
+    <row r="664" spans="1:5">
+      <c r="B664" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C664" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D664" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E664" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="665" spans="1:5">
+      <c r="B665" s="8">
+        <v>1</v>
+      </c>
+      <c r="C665" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="D665" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E665" s="8" t="s">
+        <v>796</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="165">
+  <mergeCells count="175">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B11:E11"/>
@@ -8584,6 +8979,16 @@
     <mergeCell ref="B625:E625"/>
     <mergeCell ref="B626:E626"/>
     <mergeCell ref="B627:E627"/>
+    <mergeCell ref="B634:E634"/>
+    <mergeCell ref="B635:E635"/>
+    <mergeCell ref="B636:E636"/>
+    <mergeCell ref="B643:E643"/>
+    <mergeCell ref="B644:E644"/>
+    <mergeCell ref="B645:E645"/>
+    <mergeCell ref="B652:E652"/>
+    <mergeCell ref="B653:E653"/>
+    <mergeCell ref="B661:E661"/>
+    <mergeCell ref="B662:E662"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8591,7 +8996,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D196"/>
+  <dimension ref="A2:D207"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9763,51 +10168,51 @@
         <v>441</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B137" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="C137" s="5"/>
-      <c r="D137" s="5"/>
+    <row r="136" spans="1:4">
+      <c r="B136" s="8">
+        <v>4</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B138" s="6" t="s">
-        <v>573</v>
-      </c>
-      <c r="C138" s="6"/>
-      <c r="D138" s="6"/>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="B140" s="7" t="s">
+      <c r="B139" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="B141" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C140" s="7" t="s">
+      <c r="C141" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D140" s="7" t="s">
+      <c r="D141" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="B141" s="8">
-        <v>2048</v>
-      </c>
-      <c r="C141" s="8" t="s">
-        <v>574</v>
-      </c>
-      <c r="D141" s="8" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="B142" s="8">
-        <v>2054</v>
+        <v>2048</v>
       </c>
       <c r="C142" s="8" t="s">
         <v>576</v>
@@ -9818,7 +10223,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="B143" s="8">
-        <v>34525</v>
+        <v>2054</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>578</v>
@@ -9829,7 +10234,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="B144" s="8">
-        <v>34887</v>
+        <v>34525</v>
       </c>
       <c r="C144" s="8" t="s">
         <v>580</v>
@@ -9838,51 +10243,51 @@
         <v>581</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
-      <c r="A146" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B146" s="5" t="s">
+    <row r="145" spans="1:4">
+      <c r="B145" s="8">
+        <v>34887</v>
+      </c>
+      <c r="C145" s="8" t="s">
         <v>582</v>
       </c>
-      <c r="C146" s="5"/>
-      <c r="D146" s="5"/>
+      <c r="D145" s="8" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B147" s="6" t="s">
-        <v>583</v>
-      </c>
-      <c r="C147" s="6"/>
-      <c r="D147" s="6"/>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="B149" s="7" t="s">
+      <c r="B148" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="B150" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C149" s="7" t="s">
+      <c r="C150" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D149" s="7" t="s">
+      <c r="D150" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="B150" s="8">
-        <v>1</v>
-      </c>
-      <c r="C150" s="8" t="s">
-        <v>584</v>
-      </c>
-      <c r="D150" s="8" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="B151" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C151" s="8" t="s">
         <v>586</v>
@@ -9893,7 +10298,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="B152" s="8">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C152" s="8" t="s">
         <v>588</v>
@@ -9902,51 +10307,51 @@
         <v>589</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
-      <c r="A154" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B154" s="5" t="s">
+    <row r="153" spans="1:4">
+      <c r="B153" s="8">
+        <v>17</v>
+      </c>
+      <c r="C153" s="8" t="s">
         <v>590</v>
       </c>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5"/>
+      <c r="D153" s="8" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B155" s="6" t="s">
-        <v>591</v>
-      </c>
-      <c r="C155" s="6"/>
-      <c r="D155" s="6"/>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="B157" s="7" t="s">
+      <c r="B156" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="B158" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C157" s="7" t="s">
+      <c r="C158" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D157" s="7" t="s">
+      <c r="D158" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="B158" s="8">
-        <v>20</v>
-      </c>
-      <c r="C158" s="8" t="s">
-        <v>592</v>
-      </c>
-      <c r="D158" s="8" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="B159" s="8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>594</v>
@@ -9957,7 +10362,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="B160" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>596</v>
@@ -9968,7 +10373,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="B161" s="8">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C161" s="8" t="s">
         <v>598</v>
@@ -9979,7 +10384,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="B162" s="8">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C162" s="8" t="s">
         <v>600</v>
@@ -9990,7 +10395,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="B163" s="8">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="C163" s="8" t="s">
         <v>602</v>
@@ -10001,7 +10406,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="B164" s="8">
-        <v>443</v>
+        <v>80</v>
       </c>
       <c r="C164" s="8" t="s">
         <v>604</v>
@@ -10010,41 +10415,41 @@
         <v>605</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
-      <c r="A166" s="4" t="s">
+    <row r="165" spans="1:4">
+      <c r="B165" s="8">
+        <v>443</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="D165" s="8" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B166" s="5" t="s">
-        <v>683</v>
-      </c>
-      <c r="C166" s="5"/>
-      <c r="D166" s="5"/>
-    </row>
-    <row r="168" spans="1:4">
-      <c r="B168" s="7" t="s">
+      <c r="B167" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="B169" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C168" s="7" t="s">
+      <c r="C169" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D168" s="7" t="s">
+      <c r="D169" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
-      <c r="B169" s="8">
-        <v>1</v>
-      </c>
-      <c r="C169" s="8" t="s">
-        <v>684</v>
-      </c>
-      <c r="D169" s="8" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="B170" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C170" s="8" t="s">
         <v>686</v>
@@ -10055,7 +10460,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="B171" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>688</v>
@@ -10066,7 +10471,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="B172" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>690</v>
@@ -10077,7 +10482,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="B173" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C173" s="8" t="s">
         <v>692</v>
@@ -10088,7 +10493,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="B174" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C174" s="8" t="s">
         <v>694</v>
@@ -10099,7 +10504,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="B175" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>696</v>
@@ -10110,7 +10515,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="B176" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C176" s="8" t="s">
         <v>698</v>
@@ -10121,7 +10526,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="B177" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C177" s="8" t="s">
         <v>700</v>
@@ -10132,7 +10537,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="B178" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C178" s="8" t="s">
         <v>702</v>
@@ -10143,7 +10548,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="B179" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C179" s="8" t="s">
         <v>704</v>
@@ -10152,41 +10557,41 @@
         <v>705</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
-      <c r="A181" s="4" t="s">
+    <row r="180" spans="1:4">
+      <c r="B180" s="8">
+        <v>11</v>
+      </c>
+      <c r="C180" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B181" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="C181" s="5"/>
-      <c r="D181" s="5"/>
-    </row>
-    <row r="183" spans="1:4">
-      <c r="B183" s="7" t="s">
+      <c r="B182" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="B184" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C183" s="7" t="s">
+      <c r="C184" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D183" s="7" t="s">
+      <c r="D184" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
-      <c r="B184" s="8">
-        <v>0</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>727</v>
-      </c>
-      <c r="D184" s="8" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="B185" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C185" s="8" t="s">
         <v>729</v>
@@ -10197,7 +10602,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="B186" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C186" s="8" t="s">
         <v>731</v>
@@ -10208,7 +10613,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="B187" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C187" s="8" t="s">
         <v>733</v>
@@ -10219,7 +10624,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="B188" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C188" s="8" t="s">
         <v>735</v>
@@ -10230,7 +10635,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="B189" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C189" s="8" t="s">
         <v>737</v>
@@ -10241,7 +10646,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="B190" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C190" s="8" t="s">
         <v>739</v>
@@ -10252,7 +10657,7 @@
     </row>
     <row r="191" spans="1:4">
       <c r="B191" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C191" s="8" t="s">
         <v>741</v>
@@ -10263,7 +10668,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="B192" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C192" s="8" t="s">
         <v>743</v>
@@ -10272,9 +10677,9 @@
         <v>744</v>
       </c>
     </row>
-    <row r="193" spans="2:4">
+    <row r="193" spans="1:4">
       <c r="B193" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C193" s="8" t="s">
         <v>745</v>
@@ -10283,9 +10688,9 @@
         <v>746</v>
       </c>
     </row>
-    <row r="194" spans="2:4">
+    <row r="194" spans="1:4">
       <c r="B194" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C194" s="8" t="s">
         <v>747</v>
@@ -10294,9 +10699,9 @@
         <v>748</v>
       </c>
     </row>
-    <row r="195" spans="2:4">
+    <row r="195" spans="1:4">
       <c r="B195" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C195" s="8" t="s">
         <v>749</v>
@@ -10305,9 +10710,9 @@
         <v>750</v>
       </c>
     </row>
-    <row r="196" spans="2:4">
+    <row r="196" spans="1:4">
       <c r="B196" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C196" s="8" t="s">
         <v>751</v>
@@ -10316,8 +10721,105 @@
         <v>752</v>
       </c>
     </row>
+    <row r="197" spans="1:4">
+      <c r="B197" s="8">
+        <v>12</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="D197" s="8" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="C200" s="6"/>
+      <c r="D200" s="6"/>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="B202" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C202" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D202" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="B203" s="8">
+        <v>1</v>
+      </c>
+      <c r="C203" s="8" t="s">
+        <v>769</v>
+      </c>
+      <c r="D203" s="8" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="B204" s="8">
+        <v>2</v>
+      </c>
+      <c r="C204" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="D204" s="8" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="B205" s="8">
+        <v>3</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>773</v>
+      </c>
+      <c r="D205" s="8" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="B206" s="8">
+        <v>4</v>
+      </c>
+      <c r="C206" s="8" t="s">
+        <v>775</v>
+      </c>
+      <c r="D206" s="8" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="B207" s="8">
+        <v>5</v>
+      </c>
+      <c r="C207" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="D207" s="8" t="s">
+        <v>778</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B45:D45"/>
@@ -10333,14 +10835,16 @@
     <mergeCell ref="B106:D106"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B137:D137"/>
     <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B146:D146"/>
+    <mergeCell ref="B139:D139"/>
     <mergeCell ref="B147:D147"/>
-    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="B148:D148"/>
     <mergeCell ref="B155:D155"/>
-    <mergeCell ref="B166:D166"/>
-    <mergeCell ref="B181:D181"/>
+    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="B182:D182"/>
+    <mergeCell ref="B199:D199"/>
+    <mergeCell ref="B200:D200"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add example commands and unit tests
</commit_message>
<xml_diff>
--- a/schema_gen/openc2_genj.xlsx
+++ b/schema_gen/openc2_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="849">
-  <si>
-    <t>Generated from schema\openc2.jaen, Fri Jun 23 10:34:26 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="855">
+  <si>
+    <t>Generated from schema\openc2.jaen, Wed Jun 28 16:34:53 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1386,9 +1386,15 @@
     <t>f</t>
   </si>
   <si>
+    <t>CybOX 2.1   TODO: Finish</t>
+  </si>
+  <si>
     <t>disk-partition</t>
   </si>
   <si>
+    <t>CybOX 2.1    TODO: Finish</t>
+  </si>
+  <si>
     <t>domain-name</t>
   </si>
   <si>
@@ -1707,18 +1713,12 @@
     <t>IPv4 address or range in CIDR notation</t>
   </si>
   <si>
-    <t>resolves_to_refs (optional)</t>
-  </si>
-  <si>
     <t>mac-addrs (Array)</t>
   </si>
   <si>
     <t>Specifies a list of references to one or more Layer 2 Media Access Control (MAC) addresses that the IPv4 address resolves to.</t>
   </si>
   <si>
-    <t>belongs_to_refs (optional)</t>
-  </si>
-  <si>
     <t>asystems (Array)</t>
   </si>
   <si>
@@ -2212,6 +2212,24 @@
   </si>
   <si>
     <t>user-session</t>
+  </si>
+  <si>
+    <t>effective-group (optional)</t>
+  </si>
+  <si>
+    <t>effective-group-id (optional)</t>
+  </si>
+  <si>
+    <t>effective-user (optional)</t>
+  </si>
+  <si>
+    <t>effective-user-id (optional)</t>
+  </si>
+  <si>
+    <t>login-time (optional)</t>
+  </si>
+  <si>
+    <t>logout-time (optional)</t>
   </si>
   <si>
     <t>windows-registry-key</t>
@@ -3046,7 +3064,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E739"/>
+  <dimension ref="A2:E745"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5871,7 +5889,7 @@
         <v>126</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>135</v>
+        <v>456</v>
       </c>
       <c r="C292" s="6"/>
       <c r="D292" s="6"/>
@@ -5896,7 +5914,7 @@
         <v>15</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C297" s="5"/>
       <c r="D297" s="5"/>
@@ -5918,7 +5936,7 @@
         <v>126</v>
       </c>
       <c r="B299" s="6" t="s">
-        <v>135</v>
+        <v>458</v>
       </c>
       <c r="C299" s="6"/>
       <c r="D299" s="6"/>
@@ -5943,7 +5961,7 @@
         <v>15</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C304" s="5"/>
       <c r="D304" s="5"/>
@@ -5979,13 +5997,13 @@
         <v>1</v>
       </c>
       <c r="C308" s="8" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D308" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E308" s="8" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="309" spans="1:5">
@@ -5993,13 +6011,13 @@
         <v>2</v>
       </c>
       <c r="C309" s="8" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D309" s="8" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="E309" s="8" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="312" spans="1:5">
@@ -6007,7 +6025,7 @@
         <v>15</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C312" s="5"/>
       <c r="D312" s="5"/>
@@ -6030,7 +6048,7 @@
       </c>
       <c r="C314" s="8"/>
       <c r="D314" s="8" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E314" s="8"/>
     </row>
@@ -6039,7 +6057,7 @@
         <v>15</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C317" s="5"/>
       <c r="D317" s="5"/>
@@ -6075,7 +6093,7 @@
         <v>1</v>
       </c>
       <c r="C321" s="8" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D321" s="8" t="s">
         <v>151</v>
@@ -6087,7 +6105,7 @@
         <v>2</v>
       </c>
       <c r="C322" s="8" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D322" s="8" t="s">
         <v>153</v>
@@ -6099,7 +6117,7 @@
         <v>3</v>
       </c>
       <c r="C323" s="8" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D323" s="8" t="s">
         <v>143</v>
@@ -6111,7 +6129,7 @@
         <v>15</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C326" s="5"/>
       <c r="D326" s="5"/>
@@ -6147,13 +6165,13 @@
         <v>1</v>
       </c>
       <c r="C330" s="8" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D330" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E330" s="8" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="331" spans="1:5">
@@ -6161,13 +6179,13 @@
         <v>2</v>
       </c>
       <c r="C331" s="8" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D331" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E331" s="8" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="332" spans="1:5">
@@ -6175,13 +6193,13 @@
         <v>3</v>
       </c>
       <c r="C332" s="8" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D332" s="8" t="s">
         <v>168</v>
       </c>
       <c r="E332" s="8" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="335" spans="1:5">
@@ -6189,7 +6207,7 @@
         <v>15</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C335" s="5"/>
       <c r="D335" s="5"/>
@@ -6221,7 +6239,7 @@
         <v>15</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C340" s="5"/>
       <c r="D340" s="5"/>
@@ -6253,7 +6271,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C345" s="5"/>
       <c r="D345" s="5"/>
@@ -6275,7 +6293,7 @@
         <v>126</v>
       </c>
       <c r="B347" s="6" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C347" s="6"/>
       <c r="D347" s="6"/>
@@ -6300,7 +6318,7 @@
         <v>15</v>
       </c>
       <c r="B352" s="5" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C352" s="5"/>
       <c r="D352" s="5"/>
@@ -6323,7 +6341,7 @@
       </c>
       <c r="C354" s="8"/>
       <c r="D354" s="8" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E354" s="8"/>
     </row>
@@ -6332,7 +6350,7 @@
         <v>15</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C357" s="5"/>
       <c r="D357" s="5"/>
@@ -6368,13 +6386,13 @@
         <v>1</v>
       </c>
       <c r="C361" s="8" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D361" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E361" s="8" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="362" spans="1:5">
@@ -6382,13 +6400,13 @@
         <v>2</v>
       </c>
       <c r="C362" s="8" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D362" s="8" t="s">
         <v>232</v>
       </c>
       <c r="E362" s="8" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="363" spans="1:5">
@@ -6396,13 +6414,13 @@
         <v>3</v>
       </c>
       <c r="C363" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D363" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E363" s="8" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="364" spans="1:5">
@@ -6410,13 +6428,13 @@
         <v>4</v>
       </c>
       <c r="C364" s="8" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D364" s="8" t="s">
         <v>145</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="365" spans="1:5">
@@ -6424,13 +6442,13 @@
         <v>5</v>
       </c>
       <c r="C365" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D365" s="8" t="s">
         <v>145</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="366" spans="1:5">
@@ -6438,13 +6456,13 @@
         <v>6</v>
       </c>
       <c r="C366" s="8" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D366" s="8" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="367" spans="1:5">
@@ -6452,13 +6470,13 @@
         <v>7</v>
       </c>
       <c r="C367" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="D367" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="D367" s="8" t="s">
-        <v>494</v>
-      </c>
       <c r="E367" s="8" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="368" spans="1:5">
@@ -6466,13 +6484,13 @@
         <v>8</v>
       </c>
       <c r="C368" s="8" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D368" s="8" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="369" spans="1:5">
@@ -6480,13 +6498,13 @@
         <v>9</v>
       </c>
       <c r="C369" s="8" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D369" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="370" spans="1:5">
@@ -6494,13 +6512,13 @@
         <v>10</v>
       </c>
       <c r="C370" s="8" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D370" s="8" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="371" spans="1:5">
@@ -6508,13 +6526,13 @@
         <v>11</v>
       </c>
       <c r="C371" s="8" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D371" s="8" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E371" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="372" spans="1:5">
@@ -6522,13 +6540,13 @@
         <v>12</v>
       </c>
       <c r="C372" s="8" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="D372" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="373" spans="1:5">
@@ -6536,13 +6554,13 @@
         <v>13</v>
       </c>
       <c r="C373" s="8" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D373" s="8" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E373" s="8" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="374" spans="1:5">
@@ -6550,13 +6568,13 @@
         <v>14</v>
       </c>
       <c r="C374" s="8" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D374" s="8" t="s">
         <v>129</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="377" spans="1:5">
@@ -6600,13 +6618,13 @@
         <v>1</v>
       </c>
       <c r="C381" s="8" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D381" s="8" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E381" s="8" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="382" spans="1:5">
@@ -6620,7 +6638,7 @@
         <v>415</v>
       </c>
       <c r="E382" s="8" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="383" spans="1:5">
@@ -6628,13 +6646,13 @@
         <v>3</v>
       </c>
       <c r="C383" s="8" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D383" s="8" t="s">
         <v>424</v>
       </c>
       <c r="E383" s="8" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="384" spans="1:5">
@@ -6648,7 +6666,7 @@
         <v>43</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="385" spans="1:5">
@@ -6656,13 +6674,13 @@
         <v>5</v>
       </c>
       <c r="C385" s="8" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D385" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E385" s="8" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="386" spans="1:5">
@@ -6670,13 +6688,13 @@
         <v>6</v>
       </c>
       <c r="C386" s="8" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D386" s="8" t="s">
         <v>341</v>
       </c>
       <c r="E386" s="8" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="387" spans="1:5">
@@ -6690,7 +6708,7 @@
         <v>43</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="388" spans="1:5">
@@ -6704,7 +6722,7 @@
         <v>232</v>
       </c>
       <c r="E388" s="8" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="389" spans="1:5">
@@ -6718,7 +6736,7 @@
         <v>232</v>
       </c>
       <c r="E389" s="8" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="390" spans="1:5">
@@ -6732,7 +6750,7 @@
         <v>232</v>
       </c>
       <c r="E390" s="8" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="391" spans="1:5">
@@ -6740,13 +6758,13 @@
         <v>11</v>
       </c>
       <c r="C391" s="8" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D391" s="8" t="s">
         <v>137</v>
       </c>
       <c r="E391" s="8" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="392" spans="1:5">
@@ -6754,13 +6772,13 @@
         <v>12</v>
       </c>
       <c r="C392" s="8" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E392" s="8" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="393" spans="1:5">
@@ -6768,13 +6786,13 @@
         <v>13</v>
       </c>
       <c r="C393" s="8" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D393" s="8" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E393" s="8" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="394" spans="1:5">
@@ -6782,13 +6800,13 @@
         <v>14</v>
       </c>
       <c r="C394" s="8" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D394" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E394" s="8" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="395" spans="1:5">
@@ -6799,10 +6817,10 @@
         <v>447</v>
       </c>
       <c r="D395" s="8" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E395" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="396" spans="1:5">
@@ -6810,13 +6828,13 @@
         <v>16</v>
       </c>
       <c r="C396" s="8" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D396" s="8" t="s">
         <v>129</v>
       </c>
       <c r="E396" s="8" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="399" spans="1:5">
@@ -6824,7 +6842,7 @@
         <v>15</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C399" s="5"/>
       <c r="D399" s="5"/>
@@ -6856,7 +6874,7 @@
         <v>15</v>
       </c>
       <c r="B404" s="5" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C404" s="5"/>
       <c r="D404" s="5"/>
@@ -6892,10 +6910,10 @@
         <v>1</v>
       </c>
       <c r="C408" s="8" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D408" s="8" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E408" s="8"/>
     </row>
@@ -6904,10 +6922,10 @@
         <v>2</v>
       </c>
       <c r="C409" s="8" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D409" s="8" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E409" s="8"/>
     </row>
@@ -6916,10 +6934,10 @@
         <v>3</v>
       </c>
       <c r="C410" s="8" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="D410" s="8" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E410" s="8"/>
     </row>
@@ -6928,10 +6946,10 @@
         <v>4</v>
       </c>
       <c r="C411" s="8" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D411" s="8" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E411" s="8"/>
     </row>
@@ -6940,10 +6958,10 @@
         <v>5</v>
       </c>
       <c r="C412" s="8" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D412" s="8" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E412" s="8"/>
     </row>
@@ -6952,7 +6970,7 @@
         <v>15</v>
       </c>
       <c r="B415" s="5" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C415" s="5"/>
       <c r="D415" s="5"/>
@@ -6974,7 +6992,7 @@
         <v>126</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C417" s="6"/>
       <c r="D417" s="6"/>
@@ -6999,7 +7017,7 @@
         <v>15</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="C422" s="5"/>
       <c r="D422" s="5"/>
@@ -7021,7 +7039,7 @@
         <v>126</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C424" s="6"/>
       <c r="D424" s="6"/>
@@ -7046,7 +7064,7 @@
         <v>15</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C429" s="5"/>
       <c r="D429" s="5"/>
@@ -7068,7 +7086,7 @@
         <v>126</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C431" s="6"/>
       <c r="D431" s="6"/>
@@ -7093,7 +7111,7 @@
         <v>15</v>
       </c>
       <c r="B436" s="5" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C436" s="5"/>
       <c r="D436" s="5"/>
@@ -7115,7 +7133,7 @@
         <v>126</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C438" s="6"/>
       <c r="D438" s="6"/>
@@ -7140,7 +7158,7 @@
         <v>15</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C443" s="5"/>
       <c r="D443" s="5"/>
@@ -7162,7 +7180,7 @@
         <v>126</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C445" s="6"/>
       <c r="D445" s="6"/>
@@ -7187,7 +7205,7 @@
         <v>15</v>
       </c>
       <c r="B450" s="5" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C450" s="5"/>
       <c r="D450" s="5"/>
@@ -7223,13 +7241,13 @@
         <v>1</v>
       </c>
       <c r="C454" s="8" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D454" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E454" s="8" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="455" spans="1:5">
@@ -7237,13 +7255,13 @@
         <v>2</v>
       </c>
       <c r="C455" s="8" t="s">
-        <v>563</v>
+        <v>462</v>
       </c>
       <c r="D455" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E455" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="456" spans="1:5">
@@ -7251,7 +7269,7 @@
         <v>3</v>
       </c>
       <c r="C456" s="8" t="s">
-        <v>566</v>
+        <v>475</v>
       </c>
       <c r="D456" s="8" t="s">
         <v>567</v>
@@ -7301,7 +7319,7 @@
         <v>1</v>
       </c>
       <c r="C463" s="8" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D463" s="8" t="s">
         <v>43</v>
@@ -7315,13 +7333,13 @@
         <v>2</v>
       </c>
       <c r="C464" s="8" t="s">
-        <v>563</v>
+        <v>462</v>
       </c>
       <c r="D464" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E464" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="465" spans="1:5">
@@ -7329,7 +7347,7 @@
         <v>3</v>
       </c>
       <c r="C465" s="8" t="s">
-        <v>566</v>
+        <v>475</v>
       </c>
       <c r="D465" s="8" t="s">
         <v>567</v>
@@ -7490,7 +7508,7 @@
         <v>578</v>
       </c>
       <c r="D488" s="8" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E488" s="8" t="s">
         <v>579</v>
@@ -7518,7 +7536,7 @@
         <v>583</v>
       </c>
       <c r="D490" s="8" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E490" s="8" t="s">
         <v>584</v>
@@ -7715,7 +7733,7 @@
         <v>1</v>
       </c>
       <c r="C515" s="8" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D515" s="8" t="s">
         <v>631</v>
@@ -7732,7 +7750,7 @@
         <v>633</v>
       </c>
       <c r="D516" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E516" s="8" t="s">
         <v>634</v>
@@ -8107,7 +8125,7 @@
         <v>126</v>
       </c>
       <c r="B560" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C560" s="6"/>
       <c r="D560" s="6"/>
@@ -8154,7 +8172,7 @@
         <v>126</v>
       </c>
       <c r="B567" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C567" s="6"/>
       <c r="D567" s="6"/>
@@ -8396,7 +8414,7 @@
         <v>4</v>
       </c>
       <c r="C595" s="8" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D595" s="8" t="s">
         <v>43</v>
@@ -8413,7 +8431,7 @@
         <v>690</v>
       </c>
       <c r="D596" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E596" s="8" t="s">
         <v>691</v>
@@ -8427,7 +8445,7 @@
         <v>692</v>
       </c>
       <c r="D597" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E597" s="8" t="s">
         <v>693</v>
@@ -8441,7 +8459,7 @@
         <v>694</v>
       </c>
       <c r="D598" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E598" s="8" t="s">
         <v>695</v>
@@ -8455,7 +8473,7 @@
         <v>696</v>
       </c>
       <c r="D599" s="8" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E599" s="8" t="s">
         <v>697</v>
@@ -8578,70 +8596,106 @@
         <v>21</v>
       </c>
     </row>
+    <row r="612" spans="1:5">
+      <c r="B612" s="8">
+        <v>1</v>
+      </c>
+      <c r="C612" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="D612" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E612" s="8"/>
+    </row>
+    <row r="613" spans="1:5">
+      <c r="B613" s="8">
+        <v>2</v>
+      </c>
+      <c r="C613" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="D613" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E613" s="8"/>
+    </row>
     <row r="614" spans="1:5">
-      <c r="A614" s="4" t="s">
+      <c r="B614" s="8">
+        <v>3</v>
+      </c>
+      <c r="C614" s="8" t="s">
+        <v>734</v>
+      </c>
+      <c r="D614" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E614" s="8"/>
+    </row>
+    <row r="615" spans="1:5">
+      <c r="B615" s="8">
+        <v>4</v>
+      </c>
+      <c r="C615" s="8" t="s">
+        <v>735</v>
+      </c>
+      <c r="D615" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E615" s="8"/>
+    </row>
+    <row r="616" spans="1:5">
+      <c r="B616" s="8">
+        <v>5</v>
+      </c>
+      <c r="C616" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="D616" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E616" s="8"/>
+    </row>
+    <row r="617" spans="1:5">
+      <c r="B617" s="8">
+        <v>6</v>
+      </c>
+      <c r="C617" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="D617" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E617" s="8"/>
+    </row>
+    <row r="620" spans="1:5">
+      <c r="A620" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B614" s="5" t="s">
+      <c r="B620" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C614" s="5"/>
-      <c r="D614" s="5"/>
-      <c r="E614" s="5"/>
-    </row>
-    <row r="615" spans="1:5">
-      <c r="A615" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B615" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C615" s="6"/>
-      <c r="D615" s="6"/>
-      <c r="E615" s="6"/>
-    </row>
-    <row r="616" spans="1:5">
-      <c r="A616" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B616" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C616" s="6"/>
-      <c r="D616" s="6"/>
-      <c r="E616" s="6"/>
-    </row>
-    <row r="618" spans="1:5">
-      <c r="B618" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C618" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D618" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E618" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="C620" s="5"/>
+      <c r="D620" s="5"/>
+      <c r="E620" s="5"/>
     </row>
     <row r="621" spans="1:5">
       <c r="A621" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B621" s="5" t="s">
-        <v>732</v>
-      </c>
-      <c r="C621" s="5"/>
-      <c r="D621" s="5"/>
-      <c r="E621" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B621" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C621" s="6"/>
+      <c r="D621" s="6"/>
+      <c r="E621" s="6"/>
     </row>
     <row r="622" spans="1:5">
       <c r="A622" s="4" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="B622" s="6" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C622" s="6"/>
       <c r="D622" s="6"/>
@@ -8661,967 +8715,1003 @@
         <v>21</v>
       </c>
     </row>
-    <row r="625" spans="1:5">
-      <c r="B625" s="8">
+    <row r="627" spans="1:5">
+      <c r="A627" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B627" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="C627" s="5"/>
+      <c r="D627" s="5"/>
+      <c r="E627" s="5"/>
+    </row>
+    <row r="628" spans="1:5">
+      <c r="A628" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B628" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C628" s="6"/>
+      <c r="D628" s="6"/>
+      <c r="E628" s="6"/>
+    </row>
+    <row r="630" spans="1:5">
+      <c r="B630" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C630" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D630" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E630" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="631" spans="1:5">
+      <c r="B631" s="8">
         <v>1</v>
       </c>
-      <c r="C625" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="D625" s="8" t="s">
+      <c r="C631" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="D631" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E625" s="8" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="626" spans="1:5">
-      <c r="B626" s="8">
+      <c r="E631" s="8" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5">
+      <c r="B632" s="8">
         <v>2</v>
       </c>
-      <c r="C626" s="8" t="s">
-        <v>735</v>
-      </c>
-      <c r="D626" s="8" t="s">
-        <v>736</v>
-      </c>
-      <c r="E626" s="8" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="627" spans="1:5">
-      <c r="B627" s="8">
+      <c r="C632" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="D632" s="8" t="s">
+        <v>742</v>
+      </c>
+      <c r="E632" s="8" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="633" spans="1:5">
+      <c r="B633" s="8">
         <v>3</v>
       </c>
-      <c r="C627" s="8" t="s">
+      <c r="C633" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="D627" s="8" t="s">
+      <c r="D633" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="E627" s="8" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="628" spans="1:5">
-      <c r="B628" s="8">
-        <v>4</v>
-      </c>
-      <c r="C628" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="D628" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E628" s="8" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="629" spans="1:5">
-      <c r="B629" s="8">
-        <v>5</v>
-      </c>
-      <c r="C629" s="8" t="s">
-        <v>740</v>
-      </c>
-      <c r="D629" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="E629" s="8" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="632" spans="1:5">
-      <c r="A632" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B632" s="5" t="s">
-        <v>742</v>
-      </c>
-      <c r="C632" s="5"/>
-      <c r="D632" s="5"/>
-      <c r="E632" s="5"/>
-    </row>
-    <row r="633" spans="1:5">
-      <c r="A633" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B633" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="C633" s="6"/>
-      <c r="D633" s="6"/>
-      <c r="E633" s="6"/>
+      <c r="E633" s="8" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="634" spans="1:5">
       <c r="B634" s="8">
-        <v>0</v>
-      </c>
-      <c r="C634" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C634" s="8" t="s">
+        <v>650</v>
+      </c>
       <c r="D634" s="8" t="s">
-        <v>743</v>
-      </c>
-      <c r="E634" s="8"/>
-    </row>
-    <row r="637" spans="1:5">
-      <c r="A637" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B637" s="5" t="s">
-        <v>744</v>
-      </c>
-      <c r="C637" s="5"/>
-      <c r="D637" s="5"/>
-      <c r="E637" s="5"/>
+        <v>168</v>
+      </c>
+      <c r="E634" s="8" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="635" spans="1:5">
+      <c r="B635" s="8">
+        <v>5</v>
+      </c>
+      <c r="C635" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="D635" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="E635" s="8" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="638" spans="1:5">
       <c r="A638" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B638" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="C638" s="5"/>
+      <c r="D638" s="5"/>
+      <c r="E638" s="5"/>
+    </row>
+    <row r="639" spans="1:5">
+      <c r="A639" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B638" s="6" t="s">
+      <c r="B639" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C639" s="6"/>
+      <c r="D639" s="6"/>
+      <c r="E639" s="6"/>
+    </row>
+    <row r="640" spans="1:5">
+      <c r="B640" s="8">
+        <v>0</v>
+      </c>
+      <c r="C640" s="8"/>
+      <c r="D640" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="E640" s="8"/>
+    </row>
+    <row r="643" spans="1:5">
+      <c r="A643" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B643" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C643" s="5"/>
+      <c r="D643" s="5"/>
+      <c r="E643" s="5"/>
+    </row>
+    <row r="644" spans="1:5">
+      <c r="A644" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B644" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C638" s="6"/>
-      <c r="D638" s="6"/>
-      <c r="E638" s="6"/>
-    </row>
-    <row r="640" spans="1:5">
-      <c r="B640" s="7" t="s">
+      <c r="C644" s="6"/>
+      <c r="D644" s="6"/>
+      <c r="E644" s="6"/>
+    </row>
+    <row r="646" spans="1:5">
+      <c r="B646" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C640" s="7" t="s">
+      <c r="C646" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D640" s="7" t="s">
+      <c r="D646" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E640" s="7" t="s">
+      <c r="E646" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="641" spans="1:5">
-      <c r="B641" s="8">
+    <row r="647" spans="1:5">
+      <c r="B647" s="8">
         <v>1</v>
       </c>
-      <c r="C641" s="8" t="s">
+      <c r="C647" s="8" t="s">
         <v>670</v>
       </c>
-      <c r="D641" s="8" t="s">
+      <c r="D647" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E641" s="8" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="642" spans="1:5">
-      <c r="B642" s="8">
+      <c r="E647" s="8" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="648" spans="1:5">
+      <c r="B648" s="8">
         <v>2</v>
       </c>
-      <c r="C642" s="8" t="s">
-        <v>746</v>
-      </c>
-      <c r="D642" s="8" t="s">
+      <c r="C648" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="D648" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E642" s="8" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="643" spans="1:5">
-      <c r="B643" s="8">
+      <c r="E648" s="8" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="649" spans="1:5">
+      <c r="B649" s="8">
         <v>3</v>
       </c>
-      <c r="C643" s="8" t="s">
-        <v>748</v>
-      </c>
-      <c r="D643" s="8" t="s">
-        <v>749</v>
-      </c>
-      <c r="E643" s="8" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="646" spans="1:5">
-      <c r="A646" s="4" t="s">
+      <c r="C649" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="D649" s="8" t="s">
+        <v>755</v>
+      </c>
+      <c r="E649" s="8" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="652" spans="1:5">
+      <c r="A652" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B646" s="5" t="s">
-        <v>778</v>
-      </c>
-      <c r="C646" s="5"/>
-      <c r="D646" s="5"/>
-      <c r="E646" s="5"/>
-    </row>
-    <row r="647" spans="1:5">
-      <c r="A647" s="4" t="s">
+      <c r="B652" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="C652" s="5"/>
+      <c r="D652" s="5"/>
+      <c r="E652" s="5"/>
+    </row>
+    <row r="653" spans="1:5">
+      <c r="A653" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B647" s="6" t="s">
+      <c r="B653" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C647" s="6"/>
-      <c r="D647" s="6"/>
-      <c r="E647" s="6"/>
-    </row>
-    <row r="648" spans="1:5">
-      <c r="A648" s="4" t="s">
+      <c r="C653" s="6"/>
+      <c r="D653" s="6"/>
+      <c r="E653" s="6"/>
+    </row>
+    <row r="654" spans="1:5">
+      <c r="A654" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B648" s="6" t="s">
-        <v>779</v>
-      </c>
-      <c r="C648" s="6"/>
-      <c r="D648" s="6"/>
-      <c r="E648" s="6"/>
-    </row>
-    <row r="650" spans="1:5">
-      <c r="B650" s="7" t="s">
+      <c r="B654" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="C654" s="6"/>
+      <c r="D654" s="6"/>
+      <c r="E654" s="6"/>
+    </row>
+    <row r="656" spans="1:5">
+      <c r="B656" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C650" s="7" t="s">
+      <c r="C656" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D650" s="7" t="s">
+      <c r="D656" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E650" s="7" t="s">
+      <c r="E656" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="651" spans="1:5">
-      <c r="B651" s="8">
+    <row r="657" spans="1:5">
+      <c r="B657" s="8">
         <v>1</v>
       </c>
-      <c r="C651" s="8" t="s">
-        <v>780</v>
-      </c>
-      <c r="D651" s="8" t="s">
-        <v>483</v>
-      </c>
-      <c r="E651" s="8" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="652" spans="1:5">
-      <c r="B652" s="8">
+      <c r="C657" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="D657" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="E657" s="8" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="658" spans="1:5">
+      <c r="B658" s="8">
         <v>2</v>
       </c>
-      <c r="C652" s="8" t="s">
-        <v>782</v>
-      </c>
-      <c r="D652" s="8" t="s">
+      <c r="C658" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="D658" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="E652" s="8" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="655" spans="1:5">
-      <c r="A655" s="4" t="s">
+      <c r="E658" s="8" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="661" spans="1:5">
+      <c r="A661" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B655" s="5" t="s">
+      <c r="B661" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C655" s="5"/>
-      <c r="D655" s="5"/>
-      <c r="E655" s="5"/>
-    </row>
-    <row r="656" spans="1:5">
-      <c r="A656" s="4" t="s">
+      <c r="C661" s="5"/>
+      <c r="D661" s="5"/>
+      <c r="E661" s="5"/>
+    </row>
+    <row r="662" spans="1:5">
+      <c r="A662" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B656" s="6" t="s">
+      <c r="B662" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C656" s="6"/>
-      <c r="D656" s="6"/>
-      <c r="E656" s="6"/>
-    </row>
-    <row r="657" spans="1:5">
-      <c r="A657" s="4" t="s">
+      <c r="C662" s="6"/>
+      <c r="D662" s="6"/>
+      <c r="E662" s="6"/>
+    </row>
+    <row r="663" spans="1:5">
+      <c r="A663" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B657" s="6" t="s">
-        <v>784</v>
-      </c>
-      <c r="C657" s="6"/>
-      <c r="D657" s="6"/>
-      <c r="E657" s="6"/>
-    </row>
-    <row r="659" spans="1:5">
-      <c r="B659" s="7" t="s">
+      <c r="B663" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="C663" s="6"/>
+      <c r="D663" s="6"/>
+      <c r="E663" s="6"/>
+    </row>
+    <row r="665" spans="1:5">
+      <c r="B665" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C659" s="7" t="s">
+      <c r="C665" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D659" s="7" t="s">
+      <c r="D665" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E659" s="7" t="s">
+      <c r="E665" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="660" spans="1:5">
-      <c r="B660" s="8">
+    <row r="666" spans="1:5">
+      <c r="B666" s="8">
         <v>1</v>
       </c>
-      <c r="C660" s="8" t="s">
-        <v>785</v>
-      </c>
-      <c r="D660" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="E660" s="8" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="661" spans="1:5">
-      <c r="B661" s="8">
+      <c r="C666" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="D666" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="E666" s="8" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="667" spans="1:5">
+      <c r="B667" s="8">
         <v>2</v>
       </c>
-      <c r="C661" s="8" t="s">
-        <v>788</v>
-      </c>
-      <c r="D661" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="E661" s="8" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="662" spans="1:5">
-      <c r="B662" s="8">
+      <c r="C667" s="8" t="s">
+        <v>794</v>
+      </c>
+      <c r="D667" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="E667" s="8" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="668" spans="1:5">
+      <c r="B668" s="8">
         <v>3</v>
       </c>
-      <c r="C662" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="D662" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="E662" s="8" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="663" spans="1:5">
-      <c r="B663" s="8">
+      <c r="C668" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="D668" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="E668" s="8" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="669" spans="1:5">
+      <c r="B669" s="8">
         <v>4</v>
       </c>
-      <c r="C663" s="8" t="s">
+      <c r="C669" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="D669" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="E669" s="8" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="670" spans="1:5">
+      <c r="B670" s="8">
+        <v>5</v>
+      </c>
+      <c r="C670" s="8" t="s">
+        <v>801</v>
+      </c>
+      <c r="D670" s="8" t="s">
         <v>792</v>
       </c>
-      <c r="D663" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="E663" s="8" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="664" spans="1:5">
-      <c r="B664" s="8">
-        <v>5</v>
-      </c>
-      <c r="C664" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="D664" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="E664" s="8" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="665" spans="1:5">
-      <c r="B665" s="8">
+      <c r="E670" s="8" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="671" spans="1:5">
+      <c r="B671" s="8">
         <v>6</v>
       </c>
-      <c r="C665" s="8" t="s">
+      <c r="C671" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D665" s="8" t="s">
+      <c r="D671" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E665" s="8" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="668" spans="1:5">
-      <c r="A668" s="4" t="s">
+      <c r="E671" s="8" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="674" spans="1:5">
+      <c r="A674" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B668" s="5" t="s">
-        <v>798</v>
-      </c>
-      <c r="C668" s="5"/>
-      <c r="D668" s="5"/>
-      <c r="E668" s="5"/>
-    </row>
-    <row r="669" spans="1:5">
-      <c r="A669" s="4" t="s">
+      <c r="B674" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C674" s="5"/>
+      <c r="D674" s="5"/>
+      <c r="E674" s="5"/>
+    </row>
+    <row r="675" spans="1:5">
+      <c r="A675" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B669" s="6" t="s">
+      <c r="B675" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C669" s="6"/>
-      <c r="D669" s="6"/>
-      <c r="E669" s="6"/>
-    </row>
-    <row r="671" spans="1:5">
-      <c r="B671" s="7" t="s">
+      <c r="C675" s="6"/>
+      <c r="D675" s="6"/>
+      <c r="E675" s="6"/>
+    </row>
+    <row r="677" spans="1:5">
+      <c r="B677" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C671" s="7" t="s">
+      <c r="C677" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D671" s="7" t="s">
+      <c r="D677" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E671" s="7" t="s">
+      <c r="E677" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="672" spans="1:5">
-      <c r="B672" s="8">
+    <row r="678" spans="1:5">
+      <c r="B678" s="8">
         <v>1</v>
       </c>
-      <c r="C672" s="8" t="s">
-        <v>799</v>
-      </c>
-      <c r="D672" s="8" t="s">
+      <c r="C678" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="D678" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E672" s="8"/>
-    </row>
-    <row r="673" spans="1:5">
-      <c r="B673" s="8">
-        <v>2</v>
-      </c>
-      <c r="C673" s="8" t="s">
-        <v>800</v>
-      </c>
-      <c r="D673" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="E673" s="8"/>
-    </row>
-    <row r="674" spans="1:5">
-      <c r="B674" s="8">
-        <v>3</v>
-      </c>
-      <c r="C674" s="8" t="s">
-        <v>801</v>
-      </c>
-      <c r="D674" s="8" t="s">
-        <v>802</v>
-      </c>
-      <c r="E674" s="8"/>
-    </row>
-    <row r="677" spans="1:5">
-      <c r="A677" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B677" s="5" t="s">
-        <v>800</v>
-      </c>
-      <c r="C677" s="5"/>
-      <c r="D677" s="5"/>
-      <c r="E677" s="5"/>
-    </row>
-    <row r="678" spans="1:5">
-      <c r="A678" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B678" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="C678" s="6"/>
-      <c r="D678" s="6"/>
-      <c r="E678" s="6"/>
+      <c r="E678" s="8"/>
     </row>
     <row r="679" spans="1:5">
       <c r="B679" s="8">
-        <v>0</v>
-      </c>
-      <c r="C679" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="C679" s="8" t="s">
+        <v>806</v>
+      </c>
       <c r="D679" s="8" t="s">
-        <v>43</v>
+        <v>505</v>
       </c>
       <c r="E679" s="8"/>
     </row>
-    <row r="682" spans="1:5">
-      <c r="A682" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B682" s="5" t="s">
-        <v>803</v>
-      </c>
-      <c r="C682" s="5"/>
-      <c r="D682" s="5"/>
-      <c r="E682" s="5"/>
+    <row r="680" spans="1:5">
+      <c r="B680" s="8">
+        <v>3</v>
+      </c>
+      <c r="C680" s="8" t="s">
+        <v>807</v>
+      </c>
+      <c r="D680" s="8" t="s">
+        <v>808</v>
+      </c>
+      <c r="E680" s="8"/>
     </row>
     <row r="683" spans="1:5">
       <c r="A683" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B683" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C683" s="6"/>
-      <c r="D683" s="6"/>
-      <c r="E683" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B683" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="C683" s="5"/>
+      <c r="D683" s="5"/>
+      <c r="E683" s="5"/>
     </row>
     <row r="684" spans="1:5">
       <c r="A684" s="4" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="B684" s="6" t="s">
-        <v>804</v>
+        <v>451</v>
       </c>
       <c r="C684" s="6"/>
       <c r="D684" s="6"/>
       <c r="E684" s="6"/>
     </row>
-    <row r="686" spans="1:5">
-      <c r="B686" s="7" t="s">
+    <row r="685" spans="1:5">
+      <c r="B685" s="8">
+        <v>0</v>
+      </c>
+      <c r="C685" s="8"/>
+      <c r="D685" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E685" s="8"/>
+    </row>
+    <row r="688" spans="1:5">
+      <c r="A688" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B688" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="C688" s="5"/>
+      <c r="D688" s="5"/>
+      <c r="E688" s="5"/>
+    </row>
+    <row r="689" spans="1:5">
+      <c r="A689" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B689" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C689" s="6"/>
+      <c r="D689" s="6"/>
+      <c r="E689" s="6"/>
+    </row>
+    <row r="690" spans="1:5">
+      <c r="A690" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B690" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C690" s="6"/>
+      <c r="D690" s="6"/>
+      <c r="E690" s="6"/>
+    </row>
+    <row r="692" spans="1:5">
+      <c r="B692" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C686" s="7" t="s">
+      <c r="C692" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D686" s="7" t="s">
+      <c r="D692" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E686" s="7" t="s">
+      <c r="E692" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="687" spans="1:5">
-      <c r="B687" s="8">
+    <row r="693" spans="1:5">
+      <c r="B693" s="8">
         <v>1</v>
       </c>
-      <c r="C687" s="8" t="s">
-        <v>805</v>
-      </c>
-      <c r="D687" s="8" t="s">
-        <v>806</v>
-      </c>
-      <c r="E687" s="8" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="688" spans="1:5">
-      <c r="B688" s="8">
+      <c r="C693" s="8" t="s">
+        <v>811</v>
+      </c>
+      <c r="D693" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="E693" s="8" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="694" spans="1:5">
+      <c r="B694" s="8">
         <v>2</v>
       </c>
-      <c r="C688" s="8" t="s">
-        <v>808</v>
-      </c>
-      <c r="D688" s="8" t="s">
-        <v>809</v>
-      </c>
-      <c r="E688" s="8" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="691" spans="1:5">
-      <c r="A691" s="4" t="s">
+      <c r="C694" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="D694" s="8" t="s">
+        <v>815</v>
+      </c>
+      <c r="E694" s="8" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="697" spans="1:5">
+      <c r="A697" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B691" s="5" t="s">
-        <v>811</v>
-      </c>
-      <c r="C691" s="5"/>
-      <c r="D691" s="5"/>
-      <c r="E691" s="5"/>
-    </row>
-    <row r="692" spans="1:5">
-      <c r="A692" s="4" t="s">
+      <c r="B697" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="C697" s="5"/>
+      <c r="D697" s="5"/>
+      <c r="E697" s="5"/>
+    </row>
+    <row r="698" spans="1:5">
+      <c r="A698" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B692" s="6" t="s">
+      <c r="B698" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C692" s="6"/>
-      <c r="D692" s="6"/>
-      <c r="E692" s="6"/>
-    </row>
-    <row r="693" spans="1:5">
-      <c r="A693" s="4" t="s">
+      <c r="C698" s="6"/>
+      <c r="D698" s="6"/>
+      <c r="E698" s="6"/>
+    </row>
+    <row r="699" spans="1:5">
+      <c r="A699" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B693" s="6" t="s">
-        <v>812</v>
-      </c>
-      <c r="C693" s="6"/>
-      <c r="D693" s="6"/>
-      <c r="E693" s="6"/>
-    </row>
-    <row r="695" spans="1:5">
-      <c r="B695" s="7" t="s">
+      <c r="B699" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C699" s="6"/>
+      <c r="D699" s="6"/>
+      <c r="E699" s="6"/>
+    </row>
+    <row r="701" spans="1:5">
+      <c r="B701" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C695" s="7" t="s">
+      <c r="C701" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D695" s="7" t="s">
+      <c r="D701" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E695" s="7" t="s">
+      <c r="E701" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="696" spans="1:5">
-      <c r="B696" s="8">
-        <v>1</v>
-      </c>
-      <c r="C696" s="8" t="s">
-        <v>805</v>
-      </c>
-      <c r="D696" s="8" t="s">
-        <v>813</v>
-      </c>
-      <c r="E696" s="8" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="697" spans="1:5">
-      <c r="B697" s="8">
-        <v>2</v>
-      </c>
-      <c r="C697" s="8" t="s">
-        <v>808</v>
-      </c>
-      <c r="D697" s="8" t="s">
-        <v>814</v>
-      </c>
-      <c r="E697" s="8" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="700" spans="1:5">
-      <c r="A700" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B700" s="5" t="s">
-        <v>815</v>
-      </c>
-      <c r="C700" s="5"/>
-      <c r="D700" s="5"/>
-      <c r="E700" s="5"/>
-    </row>
-    <row r="701" spans="1:5">
-      <c r="A701" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B701" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="C701" s="6"/>
-      <c r="D701" s="6"/>
-      <c r="E701" s="6"/>
     </row>
     <row r="702" spans="1:5">
       <c r="B702" s="8">
-        <v>0</v>
-      </c>
-      <c r="C702" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="C702" s="8" t="s">
+        <v>811</v>
+      </c>
       <c r="D702" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="E702" s="8" t="s">
         <v>813</v>
       </c>
-      <c r="E702" s="8"/>
-    </row>
-    <row r="705" spans="1:5">
-      <c r="A705" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B705" s="5" t="s">
-        <v>827</v>
-      </c>
-      <c r="C705" s="5"/>
-      <c r="D705" s="5"/>
-      <c r="E705" s="5"/>
+    </row>
+    <row r="703" spans="1:5">
+      <c r="B703" s="8">
+        <v>2</v>
+      </c>
+      <c r="C703" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="D703" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="E703" s="8" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="706" spans="1:5">
       <c r="A706" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B706" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="C706" s="5"/>
+      <c r="D706" s="5"/>
+      <c r="E706" s="5"/>
+    </row>
+    <row r="707" spans="1:5">
+      <c r="A707" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B706" s="6" t="s">
+      <c r="B707" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="C706" s="6"/>
-      <c r="D706" s="6"/>
-      <c r="E706" s="6"/>
-    </row>
-    <row r="707" spans="1:5">
-      <c r="B707" s="8">
+      <c r="C707" s="6"/>
+      <c r="D707" s="6"/>
+      <c r="E707" s="6"/>
+    </row>
+    <row r="708" spans="1:5">
+      <c r="B708" s="8">
         <v>0</v>
       </c>
-      <c r="C707" s="8"/>
-      <c r="D707" s="8" t="s">
-        <v>814</v>
-      </c>
-      <c r="E707" s="8"/>
-    </row>
-    <row r="710" spans="1:5">
-      <c r="A710" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B710" s="5" t="s">
-        <v>828</v>
-      </c>
-      <c r="C710" s="5"/>
-      <c r="D710" s="5"/>
-      <c r="E710" s="5"/>
+      <c r="C708" s="8"/>
+      <c r="D708" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="E708" s="8"/>
     </row>
     <row r="711" spans="1:5">
       <c r="A711" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B711" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C711" s="6"/>
-      <c r="D711" s="6"/>
-      <c r="E711" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B711" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="C711" s="5"/>
+      <c r="D711" s="5"/>
+      <c r="E711" s="5"/>
     </row>
     <row r="712" spans="1:5">
       <c r="A712" s="4" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="B712" s="6" t="s">
-        <v>810</v>
+        <v>451</v>
       </c>
       <c r="C712" s="6"/>
       <c r="D712" s="6"/>
       <c r="E712" s="6"/>
     </row>
-    <row r="714" spans="1:5">
-      <c r="B714" s="7" t="s">
+    <row r="713" spans="1:5">
+      <c r="B713" s="8">
+        <v>0</v>
+      </c>
+      <c r="C713" s="8"/>
+      <c r="D713" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="E713" s="8"/>
+    </row>
+    <row r="716" spans="1:5">
+      <c r="A716" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B716" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="C716" s="5"/>
+      <c r="D716" s="5"/>
+      <c r="E716" s="5"/>
+    </row>
+    <row r="717" spans="1:5">
+      <c r="A717" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B717" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C717" s="6"/>
+      <c r="D717" s="6"/>
+      <c r="E717" s="6"/>
+    </row>
+    <row r="718" spans="1:5">
+      <c r="A718" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B718" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="C718" s="6"/>
+      <c r="D718" s="6"/>
+      <c r="E718" s="6"/>
+    </row>
+    <row r="720" spans="1:5">
+      <c r="B720" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C714" s="7" t="s">
+      <c r="C720" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D714" s="7" t="s">
+      <c r="D720" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E714" s="7" t="s">
+      <c r="E720" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="715" spans="1:5">
-      <c r="B715" s="8">
+    <row r="721" spans="1:5">
+      <c r="B721" s="8">
         <v>1</v>
       </c>
-      <c r="C715" s="8" t="s">
-        <v>829</v>
-      </c>
-      <c r="D715" s="8" t="s">
-        <v>830</v>
-      </c>
-      <c r="E715" s="8" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="716" spans="1:5">
-      <c r="B716" s="8">
+      <c r="C721" s="8" t="s">
+        <v>835</v>
+      </c>
+      <c r="D721" s="8" t="s">
+        <v>836</v>
+      </c>
+      <c r="E721" s="8" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5">
+      <c r="B722" s="8">
         <v>2</v>
       </c>
-      <c r="C716" s="8" t="s">
-        <v>832</v>
-      </c>
-      <c r="D716" s="8" t="s">
-        <v>833</v>
-      </c>
-      <c r="E716" s="8" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="719" spans="1:5">
-      <c r="A719" s="4" t="s">
+      <c r="C722" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="D722" s="8" t="s">
+        <v>839</v>
+      </c>
+      <c r="E722" s="8" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="725" spans="1:5">
+      <c r="A725" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B719" s="5" t="s">
-        <v>835</v>
-      </c>
-      <c r="C719" s="5"/>
-      <c r="D719" s="5"/>
-      <c r="E719" s="5"/>
-    </row>
-    <row r="720" spans="1:5">
-      <c r="A720" s="4" t="s">
+      <c r="B725" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="C725" s="5"/>
+      <c r="D725" s="5"/>
+      <c r="E725" s="5"/>
+    </row>
+    <row r="726" spans="1:5">
+      <c r="A726" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B720" s="6" t="s">
+      <c r="B726" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C720" s="6"/>
-      <c r="D720" s="6"/>
-      <c r="E720" s="6"/>
-    </row>
-    <row r="721" spans="1:5">
-      <c r="A721" s="4" t="s">
+      <c r="C726" s="6"/>
+      <c r="D726" s="6"/>
+      <c r="E726" s="6"/>
+    </row>
+    <row r="727" spans="1:5">
+      <c r="A727" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B721" s="6" t="s">
-        <v>836</v>
-      </c>
-      <c r="C721" s="6"/>
-      <c r="D721" s="6"/>
-      <c r="E721" s="6"/>
-    </row>
-    <row r="723" spans="1:5">
-      <c r="B723" s="7" t="s">
+      <c r="B727" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="C727" s="6"/>
+      <c r="D727" s="6"/>
+      <c r="E727" s="6"/>
+    </row>
+    <row r="729" spans="1:5">
+      <c r="B729" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C723" s="7" t="s">
+      <c r="C729" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D723" s="7" t="s">
+      <c r="D729" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E723" s="7" t="s">
+      <c r="E729" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="724" spans="1:5">
-      <c r="B724" s="8">
+    <row r="730" spans="1:5">
+      <c r="B730" s="8">
         <v>1</v>
       </c>
-      <c r="C724" s="8" t="s">
-        <v>837</v>
-      </c>
-      <c r="D724" s="8" t="s">
+      <c r="C730" s="8" t="s">
+        <v>843</v>
+      </c>
+      <c r="D730" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="E724" s="8" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="725" spans="1:5">
-      <c r="B725" s="8">
+      <c r="E730" s="8" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="731" spans="1:5">
+      <c r="B731" s="8">
         <v>2</v>
       </c>
-      <c r="C725" s="8" t="s">
-        <v>839</v>
-      </c>
-      <c r="D725" s="8" t="s">
+      <c r="C731" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="D731" s="8" t="s">
         <v>588</v>
       </c>
-      <c r="E725" s="8" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="726" spans="1:5">
-      <c r="B726" s="8">
+      <c r="E731" s="8" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="732" spans="1:5">
+      <c r="B732" s="8">
         <v>3</v>
       </c>
-      <c r="C726" s="8" t="s">
-        <v>841</v>
-      </c>
-      <c r="D726" s="8" t="s">
-        <v>842</v>
-      </c>
-      <c r="E726" s="8" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="729" spans="1:5">
-      <c r="A729" s="4" t="s">
+      <c r="C732" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="D732" s="8" t="s">
+        <v>848</v>
+      </c>
+      <c r="E732" s="8" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="735" spans="1:5">
+      <c r="A735" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B729" s="5" t="s">
-        <v>844</v>
-      </c>
-      <c r="C729" s="5"/>
-      <c r="D729" s="5"/>
-      <c r="E729" s="5"/>
-    </row>
-    <row r="730" spans="1:5">
-      <c r="A730" s="4" t="s">
+      <c r="B735" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="C735" s="5"/>
+      <c r="D735" s="5"/>
+      <c r="E735" s="5"/>
+    </row>
+    <row r="736" spans="1:5">
+      <c r="A736" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B730" s="6" t="s">
+      <c r="B736" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C730" s="6"/>
-      <c r="D730" s="6"/>
-      <c r="E730" s="6"/>
-    </row>
-    <row r="731" spans="1:5">
-      <c r="A731" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B731" s="6" t="s">
-        <v>836</v>
-      </c>
-      <c r="C731" s="6"/>
-      <c r="D731" s="6"/>
-      <c r="E731" s="6"/>
-    </row>
-    <row r="733" spans="1:5">
-      <c r="B733" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C733" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D733" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E733" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="734" spans="1:5">
-      <c r="B734" s="8">
-        <v>1</v>
-      </c>
-      <c r="C734" s="8" t="s">
-        <v>845</v>
-      </c>
-      <c r="D734" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E734" s="8" t="s">
-        <v>846</v>
-      </c>
+      <c r="C736" s="6"/>
+      <c r="D736" s="6"/>
+      <c r="E736" s="6"/>
     </row>
     <row r="737" spans="1:5">
       <c r="A737" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B737" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="C737" s="6"/>
+      <c r="D737" s="6"/>
+      <c r="E737" s="6"/>
+    </row>
+    <row r="739" spans="1:5">
+      <c r="B739" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C739" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D739" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E739" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="740" spans="1:5">
+      <c r="B740" s="8">
+        <v>1</v>
+      </c>
+      <c r="C740" s="8" t="s">
+        <v>851</v>
+      </c>
+      <c r="D740" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E740" s="8" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="743" spans="1:5">
+      <c r="A743" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B737" s="5" t="s">
-        <v>847</v>
-      </c>
-      <c r="C737" s="5"/>
-      <c r="D737" s="5"/>
-      <c r="E737" s="5"/>
-    </row>
-    <row r="738" spans="1:5">
-      <c r="A738" s="4" t="s">
+      <c r="B743" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="C743" s="5"/>
+      <c r="D743" s="5"/>
+      <c r="E743" s="5"/>
+    </row>
+    <row r="744" spans="1:5">
+      <c r="A744" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B738" s="6" t="s">
+      <c r="B744" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C738" s="6"/>
-      <c r="D738" s="6"/>
-      <c r="E738" s="6"/>
-    </row>
-    <row r="739" spans="1:5">
-      <c r="A739" s="4" t="s">
+      <c r="C744" s="6"/>
+      <c r="D744" s="6"/>
+      <c r="E744" s="6"/>
+    </row>
+    <row r="745" spans="1:5">
+      <c r="A745" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B739" s="6" t="s">
-        <v>848</v>
-      </c>
-      <c r="C739" s="6"/>
-      <c r="D739" s="6"/>
-      <c r="E739" s="6"/>
+      <c r="B745" s="6" t="s">
+        <v>854</v>
+      </c>
+      <c r="C745" s="6"/>
+      <c r="D745" s="6"/>
+      <c r="E745" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="198">
@@ -9782,47 +9872,47 @@
     <mergeCell ref="B607:E607"/>
     <mergeCell ref="B608:E608"/>
     <mergeCell ref="B609:E609"/>
-    <mergeCell ref="B614:E614"/>
-    <mergeCell ref="B615:E615"/>
-    <mergeCell ref="B616:E616"/>
+    <mergeCell ref="B620:E620"/>
     <mergeCell ref="B621:E621"/>
     <mergeCell ref="B622:E622"/>
-    <mergeCell ref="B632:E632"/>
-    <mergeCell ref="B633:E633"/>
-    <mergeCell ref="B637:E637"/>
+    <mergeCell ref="B627:E627"/>
+    <mergeCell ref="B628:E628"/>
     <mergeCell ref="B638:E638"/>
-    <mergeCell ref="B646:E646"/>
-    <mergeCell ref="B647:E647"/>
-    <mergeCell ref="B648:E648"/>
-    <mergeCell ref="B655:E655"/>
-    <mergeCell ref="B656:E656"/>
-    <mergeCell ref="B657:E657"/>
-    <mergeCell ref="B668:E668"/>
-    <mergeCell ref="B669:E669"/>
-    <mergeCell ref="B677:E677"/>
-    <mergeCell ref="B678:E678"/>
-    <mergeCell ref="B682:E682"/>
+    <mergeCell ref="B639:E639"/>
+    <mergeCell ref="B643:E643"/>
+    <mergeCell ref="B644:E644"/>
+    <mergeCell ref="B652:E652"/>
+    <mergeCell ref="B653:E653"/>
+    <mergeCell ref="B654:E654"/>
+    <mergeCell ref="B661:E661"/>
+    <mergeCell ref="B662:E662"/>
+    <mergeCell ref="B663:E663"/>
+    <mergeCell ref="B674:E674"/>
+    <mergeCell ref="B675:E675"/>
     <mergeCell ref="B683:E683"/>
     <mergeCell ref="B684:E684"/>
-    <mergeCell ref="B691:E691"/>
-    <mergeCell ref="B692:E692"/>
-    <mergeCell ref="B693:E693"/>
-    <mergeCell ref="B700:E700"/>
-    <mergeCell ref="B701:E701"/>
-    <mergeCell ref="B705:E705"/>
+    <mergeCell ref="B688:E688"/>
+    <mergeCell ref="B689:E689"/>
+    <mergeCell ref="B690:E690"/>
+    <mergeCell ref="B697:E697"/>
+    <mergeCell ref="B698:E698"/>
+    <mergeCell ref="B699:E699"/>
     <mergeCell ref="B706:E706"/>
-    <mergeCell ref="B710:E710"/>
+    <mergeCell ref="B707:E707"/>
     <mergeCell ref="B711:E711"/>
     <mergeCell ref="B712:E712"/>
-    <mergeCell ref="B719:E719"/>
-    <mergeCell ref="B720:E720"/>
-    <mergeCell ref="B721:E721"/>
-    <mergeCell ref="B729:E729"/>
-    <mergeCell ref="B730:E730"/>
-    <mergeCell ref="B731:E731"/>
+    <mergeCell ref="B716:E716"/>
+    <mergeCell ref="B717:E717"/>
+    <mergeCell ref="B718:E718"/>
+    <mergeCell ref="B725:E725"/>
+    <mergeCell ref="B726:E726"/>
+    <mergeCell ref="B727:E727"/>
+    <mergeCell ref="B735:E735"/>
+    <mergeCell ref="B736:E736"/>
     <mergeCell ref="B737:E737"/>
-    <mergeCell ref="B738:E738"/>
-    <mergeCell ref="B739:E739"/>
+    <mergeCell ref="B743:E743"/>
+    <mergeCell ref="B744:E744"/>
+    <mergeCell ref="B745:E745"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11332,7 +11422,7 @@
         <v>56</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -11353,10 +11443,10 @@
         <v>0</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -11364,10 +11454,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -11375,10 +11465,10 @@
         <v>2</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -11386,10 +11476,10 @@
         <v>3</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -11397,10 +11487,10 @@
         <v>4</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -11408,10 +11498,10 @@
         <v>5</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -11419,10 +11509,10 @@
         <v>6</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -11430,10 +11520,10 @@
         <v>7</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -11441,10 +11531,10 @@
         <v>8</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -11452,10 +11542,10 @@
         <v>9</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -11463,10 +11553,10 @@
         <v>10</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -11474,10 +11564,10 @@
         <v>11</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -11485,10 +11575,10 @@
         <v>12</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>777</v>
+        <v>783</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -11496,7 +11586,7 @@
         <v>56</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -11506,7 +11596,7 @@
         <v>126</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>807</v>
+        <v>813</v>
       </c>
       <c r="C191" s="6"/>
       <c r="D191" s="6"/>
@@ -11527,10 +11617,10 @@
         <v>1</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>817</v>
+        <v>823</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>818</v>
+        <v>824</v>
       </c>
     </row>
     <row r="195" spans="2:4">
@@ -11538,10 +11628,10 @@
         <v>2</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>819</v>
+        <v>825</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>820</v>
+        <v>826</v>
       </c>
     </row>
     <row r="196" spans="2:4">
@@ -11549,10 +11639,10 @@
         <v>3</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>822</v>
+        <v>828</v>
       </c>
     </row>
     <row r="197" spans="2:4">
@@ -11560,10 +11650,10 @@
         <v>4</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>823</v>
+        <v>829</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>824</v>
+        <v>830</v>
       </c>
     </row>
     <row r="198" spans="2:4">
@@ -11571,10 +11661,10 @@
         <v>5</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>825</v>
+        <v>831</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>826</v>
+        <v>832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add query actions and query schema examples
</commit_message>
<xml_diff>
--- a/schema_gen/openc2_genj.xlsx
+++ b/schema_gen/openc2_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="855">
-  <si>
-    <t>Generated from schema\openc2.jaen, Wed Jun 28 16:34:53 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="879">
+  <si>
+    <t>Generated from schema\openc2.jaen, Wed Jul  5 11:28:02 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -2382,10 +2382,82 @@
     <t>Specifies whether the certificate is self-signed</t>
   </si>
   <si>
-    <t>hashes (required)</t>
-  </si>
-  <si>
     <t>Specifies any hashes calculated for the entire contents of the certificate</t>
+  </si>
+  <si>
+    <t>Version of the encoded certificate</t>
+  </si>
+  <si>
+    <t>Unique identifier for the certificate</t>
+  </si>
+  <si>
+    <t>signature_algorithm (optional)</t>
+  </si>
+  <si>
+    <t>Name of the algorithm used to sign the certificate</t>
+  </si>
+  <si>
+    <t>issuer (optional)</t>
+  </si>
+  <si>
+    <t>Distinguished Name of the Certification Authority that issued the certificate</t>
+  </si>
+  <si>
+    <t>validity_not_before (optional)</t>
+  </si>
+  <si>
+    <t>Date on which the validity period begins</t>
+  </si>
+  <si>
+    <t>validity_not_after (optional)</t>
+  </si>
+  <si>
+    <t>Date on which the validity period ends</t>
+  </si>
+  <si>
+    <t>Distinguished Name of the entity associated with the public key</t>
+  </si>
+  <si>
+    <t>subject_public_key_algorithm (optional)</t>
+  </si>
+  <si>
+    <t>Algorithm that uses the subject's public key</t>
+  </si>
+  <si>
+    <t>subject_public_key_modulus (optional)</t>
+  </si>
+  <si>
+    <t>Modulus of an RSA public key</t>
+  </si>
+  <si>
+    <t>subject_public_key_exponent (optional)</t>
+  </si>
+  <si>
+    <t>Exponent of an RSA public key</t>
+  </si>
+  <si>
+    <t>x509_v3_extensions (optional)</t>
+  </si>
+  <si>
+    <t>x509-v3-extensions (Array)</t>
+  </si>
+  <si>
+    <t>X.509 v3 extensions</t>
+  </si>
+  <si>
+    <t>x509-v3-extensions</t>
+  </si>
+  <si>
+    <t>x509-v3-extension (Map)</t>
+  </si>
+  <si>
+    <t>x509-v3-extension</t>
+  </si>
+  <si>
+    <t>basic_constraints (optional)</t>
+  </si>
+  <si>
+    <t>TODO: fill in extensions</t>
   </si>
   <si>
     <t>Target used to query Actuator for its supported capabilities and negotiate connection</t>
@@ -3064,7 +3136,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E745"/>
+  <dimension ref="A2:E768"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8997,323 +9069,380 @@
         <v>2</v>
       </c>
       <c r="C658" s="8" t="s">
-        <v>788</v>
+        <v>414</v>
       </c>
       <c r="D658" s="8" t="s">
         <v>415</v>
       </c>
       <c r="E658" s="8" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="659" spans="1:5">
+      <c r="B659" s="8">
+        <v>3</v>
+      </c>
+      <c r="C659" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="D659" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E659" s="8" t="s">
         <v>789</v>
       </c>
     </row>
+    <row r="660" spans="1:5">
+      <c r="B660" s="8">
+        <v>4</v>
+      </c>
+      <c r="C660" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D660" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E660" s="8" t="s">
+        <v>790</v>
+      </c>
+    </row>
     <row r="661" spans="1:5">
-      <c r="A661" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B661" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C661" s="5"/>
-      <c r="D661" s="5"/>
-      <c r="E661" s="5"/>
+      <c r="B661" s="8">
+        <v>5</v>
+      </c>
+      <c r="C661" s="8" t="s">
+        <v>791</v>
+      </c>
+      <c r="D661" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E661" s="8" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="662" spans="1:5">
-      <c r="A662" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B662" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C662" s="6"/>
-      <c r="D662" s="6"/>
-      <c r="E662" s="6"/>
+      <c r="B662" s="8">
+        <v>6</v>
+      </c>
+      <c r="C662" s="8" t="s">
+        <v>793</v>
+      </c>
+      <c r="D662" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E662" s="8" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="663" spans="1:5">
-      <c r="A663" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B663" s="6" t="s">
-        <v>790</v>
-      </c>
-      <c r="C663" s="6"/>
-      <c r="D663" s="6"/>
-      <c r="E663" s="6"/>
+      <c r="B663" s="8">
+        <v>7</v>
+      </c>
+      <c r="C663" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="D663" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E663" s="8" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="664" spans="1:5">
+      <c r="B664" s="8">
+        <v>8</v>
+      </c>
+      <c r="C664" s="8" t="s">
+        <v>797</v>
+      </c>
+      <c r="D664" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E664" s="8" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="665" spans="1:5">
-      <c r="B665" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C665" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D665" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E665" s="7" t="s">
-        <v>21</v>
+      <c r="B665" s="8">
+        <v>9</v>
+      </c>
+      <c r="C665" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="D665" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E665" s="8" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="666" spans="1:5">
       <c r="B666" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C666" s="8" t="s">
-        <v>791</v>
+        <v>800</v>
       </c>
       <c r="D666" s="8" t="s">
-        <v>792</v>
+        <v>43</v>
       </c>
       <c r="E666" s="8" t="s">
-        <v>793</v>
+        <v>801</v>
       </c>
     </row>
     <row r="667" spans="1:5">
       <c r="B667" s="8">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C667" s="8" t="s">
-        <v>794</v>
+        <v>802</v>
       </c>
       <c r="D667" s="8" t="s">
-        <v>792</v>
+        <v>43</v>
       </c>
       <c r="E667" s="8" t="s">
-        <v>795</v>
+        <v>803</v>
       </c>
     </row>
     <row r="668" spans="1:5">
       <c r="B668" s="8">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C668" s="8" t="s">
-        <v>796</v>
+        <v>804</v>
       </c>
       <c r="D668" s="8" t="s">
-        <v>792</v>
+        <v>424</v>
       </c>
       <c r="E668" s="8" t="s">
-        <v>797</v>
+        <v>805</v>
       </c>
     </row>
     <row r="669" spans="1:5">
       <c r="B669" s="8">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C669" s="8" t="s">
-        <v>798</v>
+        <v>806</v>
       </c>
       <c r="D669" s="8" t="s">
-        <v>799</v>
+        <v>807</v>
       </c>
       <c r="E669" s="8" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="670" spans="1:5">
-      <c r="B670" s="8">
-        <v>5</v>
-      </c>
-      <c r="C670" s="8" t="s">
-        <v>801</v>
-      </c>
-      <c r="D670" s="8" t="s">
-        <v>792</v>
-      </c>
-      <c r="E670" s="8" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="671" spans="1:5">
-      <c r="B671" s="8">
-        <v>6</v>
-      </c>
-      <c r="C671" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D671" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E671" s="8" t="s">
-        <v>803</v>
-      </c>
+        <v>808</v>
+      </c>
+    </row>
+    <row r="672" spans="1:5">
+      <c r="A672" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B672" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="C672" s="5"/>
+      <c r="D672" s="5"/>
+      <c r="E672" s="5"/>
+    </row>
+    <row r="673" spans="1:5">
+      <c r="A673" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B673" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C673" s="6"/>
+      <c r="D673" s="6"/>
+      <c r="E673" s="6"/>
     </row>
     <row r="674" spans="1:5">
-      <c r="A674" s="4" t="s">
+      <c r="B674" s="8">
+        <v>0</v>
+      </c>
+      <c r="C674" s="8"/>
+      <c r="D674" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="E674" s="8"/>
+    </row>
+    <row r="677" spans="1:5">
+      <c r="A677" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B674" s="5" t="s">
-        <v>804</v>
-      </c>
-      <c r="C674" s="5"/>
-      <c r="D674" s="5"/>
-      <c r="E674" s="5"/>
-    </row>
-    <row r="675" spans="1:5">
-      <c r="A675" s="4" t="s">
+      <c r="B677" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="C677" s="5"/>
+      <c r="D677" s="5"/>
+      <c r="E677" s="5"/>
+    </row>
+    <row r="678" spans="1:5">
+      <c r="A678" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B675" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C675" s="6"/>
-      <c r="D675" s="6"/>
-      <c r="E675" s="6"/>
-    </row>
-    <row r="677" spans="1:5">
-      <c r="B677" s="7" t="s">
+      <c r="B678" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C678" s="6"/>
+      <c r="D678" s="6"/>
+      <c r="E678" s="6"/>
+    </row>
+    <row r="680" spans="1:5">
+      <c r="B680" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C677" s="7" t="s">
+      <c r="C680" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D677" s="7" t="s">
+      <c r="D680" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E677" s="7" t="s">
+      <c r="E680" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="678" spans="1:5">
-      <c r="B678" s="8">
+    <row r="681" spans="1:5">
+      <c r="B681" s="8">
         <v>1</v>
       </c>
-      <c r="C678" s="8" t="s">
-        <v>805</v>
-      </c>
-      <c r="D678" s="8" t="s">
+      <c r="C681" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="D681" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E678" s="8"/>
-    </row>
-    <row r="679" spans="1:5">
-      <c r="B679" s="8">
-        <v>2</v>
-      </c>
-      <c r="C679" s="8" t="s">
-        <v>806</v>
-      </c>
-      <c r="D679" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="E679" s="8"/>
-    </row>
-    <row r="680" spans="1:5">
-      <c r="B680" s="8">
-        <v>3</v>
-      </c>
-      <c r="C680" s="8" t="s">
-        <v>807</v>
-      </c>
-      <c r="D680" s="8" t="s">
-        <v>808</v>
-      </c>
-      <c r="E680" s="8"/>
-    </row>
-    <row r="683" spans="1:5">
-      <c r="A683" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B683" s="5" t="s">
-        <v>806</v>
-      </c>
-      <c r="C683" s="5"/>
-      <c r="D683" s="5"/>
-      <c r="E683" s="5"/>
+      <c r="E681" s="8" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="684" spans="1:5">
       <c r="A684" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B684" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C684" s="5"/>
+      <c r="D684" s="5"/>
+      <c r="E684" s="5"/>
+    </row>
+    <row r="685" spans="1:5">
+      <c r="A685" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B684" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="C684" s="6"/>
-      <c r="D684" s="6"/>
-      <c r="E684" s="6"/>
-    </row>
-    <row r="685" spans="1:5">
-      <c r="B685" s="8">
-        <v>0</v>
-      </c>
-      <c r="C685" s="8"/>
-      <c r="D685" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E685" s="8"/>
+      <c r="B685" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C685" s="6"/>
+      <c r="D685" s="6"/>
+      <c r="E685" s="6"/>
+    </row>
+    <row r="686" spans="1:5">
+      <c r="A686" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B686" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="C686" s="6"/>
+      <c r="D686" s="6"/>
+      <c r="E686" s="6"/>
     </row>
     <row r="688" spans="1:5">
-      <c r="A688" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B688" s="5" t="s">
-        <v>809</v>
-      </c>
-      <c r="C688" s="5"/>
-      <c r="D688" s="5"/>
-      <c r="E688" s="5"/>
+      <c r="B688" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C688" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D688" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E688" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="689" spans="1:5">
-      <c r="A689" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B689" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C689" s="6"/>
-      <c r="D689" s="6"/>
-      <c r="E689" s="6"/>
+      <c r="B689" s="8">
+        <v>1</v>
+      </c>
+      <c r="C689" s="8" t="s">
+        <v>815</v>
+      </c>
+      <c r="D689" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="E689" s="8" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="690" spans="1:5">
-      <c r="A690" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B690" s="6" t="s">
-        <v>810</v>
-      </c>
-      <c r="C690" s="6"/>
-      <c r="D690" s="6"/>
-      <c r="E690" s="6"/>
+      <c r="B690" s="8">
+        <v>2</v>
+      </c>
+      <c r="C690" s="8" t="s">
+        <v>818</v>
+      </c>
+      <c r="D690" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="E690" s="8" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="691" spans="1:5">
+      <c r="B691" s="8">
+        <v>3</v>
+      </c>
+      <c r="C691" s="8" t="s">
+        <v>820</v>
+      </c>
+      <c r="D691" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="E691" s="8" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="692" spans="1:5">
-      <c r="B692" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C692" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D692" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E692" s="7" t="s">
-        <v>21</v>
+      <c r="B692" s="8">
+        <v>4</v>
+      </c>
+      <c r="C692" s="8" t="s">
+        <v>822</v>
+      </c>
+      <c r="D692" s="8" t="s">
+        <v>823</v>
+      </c>
+      <c r="E692" s="8" t="s">
+        <v>824</v>
       </c>
     </row>
     <row r="693" spans="1:5">
       <c r="B693" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C693" s="8" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
       <c r="D693" s="8" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="E693" s="8" t="s">
-        <v>813</v>
+        <v>826</v>
       </c>
     </row>
     <row r="694" spans="1:5">
       <c r="B694" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C694" s="8" t="s">
-        <v>814</v>
+        <v>22</v>
       </c>
       <c r="D694" s="8" t="s">
-        <v>815</v>
+        <v>49</v>
       </c>
       <c r="E694" s="8" t="s">
-        <v>816</v>
+        <v>827</v>
       </c>
     </row>
     <row r="697" spans="1:5">
@@ -9321,7 +9450,7 @@
         <v>15</v>
       </c>
       <c r="B697" s="5" t="s">
-        <v>817</v>
+        <v>828</v>
       </c>
       <c r="C697" s="5"/>
       <c r="D697" s="5"/>
@@ -9332,71 +9461,68 @@
         <v>16</v>
       </c>
       <c r="B698" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C698" s="6"/>
       <c r="D698" s="6"/>
       <c r="E698" s="6"/>
     </row>
-    <row r="699" spans="1:5">
-      <c r="A699" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B699" s="6" t="s">
-        <v>818</v>
-      </c>
-      <c r="C699" s="6"/>
-      <c r="D699" s="6"/>
-      <c r="E699" s="6"/>
+    <row r="700" spans="1:5">
+      <c r="B700" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C700" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D700" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E700" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="701" spans="1:5">
-      <c r="B701" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C701" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D701" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E701" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="B701" s="8">
+        <v>1</v>
+      </c>
+      <c r="C701" s="8" t="s">
+        <v>829</v>
+      </c>
+      <c r="D701" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E701" s="8"/>
     </row>
     <row r="702" spans="1:5">
       <c r="B702" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C702" s="8" t="s">
-        <v>811</v>
+        <v>830</v>
       </c>
       <c r="D702" s="8" t="s">
-        <v>819</v>
-      </c>
-      <c r="E702" s="8" t="s">
-        <v>813</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="E702" s="8"/>
     </row>
     <row r="703" spans="1:5">
       <c r="B703" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C703" s="8" t="s">
-        <v>814</v>
+        <v>831</v>
       </c>
       <c r="D703" s="8" t="s">
-        <v>820</v>
-      </c>
-      <c r="E703" s="8" t="s">
-        <v>816</v>
-      </c>
+        <v>832</v>
+      </c>
+      <c r="E703" s="8"/>
     </row>
     <row r="706" spans="1:5">
       <c r="A706" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B706" s="5" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
       <c r="C706" s="5"/>
       <c r="D706" s="5"/>
@@ -9419,7 +9545,7 @@
       </c>
       <c r="C708" s="8"/>
       <c r="D708" s="8" t="s">
-        <v>819</v>
+        <v>43</v>
       </c>
       <c r="E708" s="8"/>
     </row>
@@ -9439,282 +9565,464 @@
         <v>16</v>
       </c>
       <c r="B712" s="6" t="s">
-        <v>451</v>
+        <v>29</v>
       </c>
       <c r="C712" s="6"/>
       <c r="D712" s="6"/>
       <c r="E712" s="6"/>
     </row>
     <row r="713" spans="1:5">
-      <c r="B713" s="8">
-        <v>0</v>
-      </c>
-      <c r="C713" s="8"/>
-      <c r="D713" s="8" t="s">
-        <v>820</v>
-      </c>
-      <c r="E713" s="8"/>
+      <c r="A713" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B713" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="C713" s="6"/>
+      <c r="D713" s="6"/>
+      <c r="E713" s="6"/>
+    </row>
+    <row r="715" spans="1:5">
+      <c r="B715" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C715" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D715" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E715" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="716" spans="1:5">
-      <c r="A716" s="4" t="s">
+      <c r="B716" s="8">
+        <v>1</v>
+      </c>
+      <c r="C716" s="8" t="s">
+        <v>835</v>
+      </c>
+      <c r="D716" s="8" t="s">
+        <v>836</v>
+      </c>
+      <c r="E716" s="8" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5">
+      <c r="B717" s="8">
+        <v>2</v>
+      </c>
+      <c r="C717" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="D717" s="8" t="s">
+        <v>839</v>
+      </c>
+      <c r="E717" s="8" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5">
+      <c r="A720" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B716" s="5" t="s">
-        <v>834</v>
-      </c>
-      <c r="C716" s="5"/>
-      <c r="D716" s="5"/>
-      <c r="E716" s="5"/>
-    </row>
-    <row r="717" spans="1:5">
-      <c r="A717" s="4" t="s">
+      <c r="B720" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="C720" s="5"/>
+      <c r="D720" s="5"/>
+      <c r="E720" s="5"/>
+    </row>
+    <row r="721" spans="1:5">
+      <c r="A721" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B717" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C717" s="6"/>
-      <c r="D717" s="6"/>
-      <c r="E717" s="6"/>
-    </row>
-    <row r="718" spans="1:5">
-      <c r="A718" s="4" t="s">
+      <c r="B721" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C721" s="6"/>
+      <c r="D721" s="6"/>
+      <c r="E721" s="6"/>
+    </row>
+    <row r="722" spans="1:5">
+      <c r="A722" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B718" s="6" t="s">
-        <v>816</v>
-      </c>
-      <c r="C718" s="6"/>
-      <c r="D718" s="6"/>
-      <c r="E718" s="6"/>
-    </row>
-    <row r="720" spans="1:5">
-      <c r="B720" s="7" t="s">
+      <c r="B722" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="C722" s="6"/>
+      <c r="D722" s="6"/>
+      <c r="E722" s="6"/>
+    </row>
+    <row r="724" spans="1:5">
+      <c r="B724" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C720" s="7" t="s">
+      <c r="C724" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D720" s="7" t="s">
+      <c r="D724" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E720" s="7" t="s">
+      <c r="E724" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="721" spans="1:5">
-      <c r="B721" s="8">
+    <row r="725" spans="1:5">
+      <c r="B725" s="8">
         <v>1</v>
       </c>
-      <c r="C721" s="8" t="s">
+      <c r="C725" s="8" t="s">
         <v>835</v>
       </c>
-      <c r="D721" s="8" t="s">
-        <v>836</v>
-      </c>
-      <c r="E721" s="8" t="s">
+      <c r="D725" s="8" t="s">
+        <v>843</v>
+      </c>
+      <c r="E725" s="8" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="722" spans="1:5">
-      <c r="B722" s="8">
+    <row r="726" spans="1:5">
+      <c r="B726" s="8">
         <v>2</v>
       </c>
-      <c r="C722" s="8" t="s">
+      <c r="C726" s="8" t="s">
         <v>838</v>
       </c>
-      <c r="D722" s="8" t="s">
-        <v>839</v>
-      </c>
-      <c r="E722" s="8" t="s">
+      <c r="D726" s="8" t="s">
+        <v>844</v>
+      </c>
+      <c r="E726" s="8" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="725" spans="1:5">
-      <c r="A725" s="4" t="s">
+    <row r="729" spans="1:5">
+      <c r="A729" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B725" s="5" t="s">
-        <v>841</v>
-      </c>
-      <c r="C725" s="5"/>
-      <c r="D725" s="5"/>
-      <c r="E725" s="5"/>
-    </row>
-    <row r="726" spans="1:5">
-      <c r="A726" s="4" t="s">
+      <c r="B729" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="C729" s="5"/>
+      <c r="D729" s="5"/>
+      <c r="E729" s="5"/>
+    </row>
+    <row r="730" spans="1:5">
+      <c r="A730" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B726" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C726" s="6"/>
-      <c r="D726" s="6"/>
-      <c r="E726" s="6"/>
-    </row>
-    <row r="727" spans="1:5">
-      <c r="A727" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B727" s="6" t="s">
-        <v>842</v>
-      </c>
-      <c r="C727" s="6"/>
-      <c r="D727" s="6"/>
-      <c r="E727" s="6"/>
-    </row>
-    <row r="729" spans="1:5">
-      <c r="B729" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C729" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D729" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E729" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="730" spans="1:5">
-      <c r="B730" s="8">
-        <v>1</v>
-      </c>
-      <c r="C730" s="8" t="s">
-        <v>843</v>
-      </c>
-      <c r="D730" s="8" t="s">
-        <v>581</v>
-      </c>
-      <c r="E730" s="8" t="s">
-        <v>844</v>
-      </c>
+      <c r="B730" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C730" s="6"/>
+      <c r="D730" s="6"/>
+      <c r="E730" s="6"/>
     </row>
     <row r="731" spans="1:5">
       <c r="B731" s="8">
-        <v>2</v>
-      </c>
-      <c r="C731" s="8" t="s">
-        <v>845</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C731" s="8"/>
       <c r="D731" s="8" t="s">
-        <v>588</v>
-      </c>
-      <c r="E731" s="8" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="732" spans="1:5">
-      <c r="B732" s="8">
-        <v>3</v>
-      </c>
-      <c r="C732" s="8" t="s">
-        <v>847</v>
-      </c>
-      <c r="D732" s="8" t="s">
-        <v>848</v>
-      </c>
-      <c r="E732" s="8" t="s">
-        <v>849</v>
-      </c>
+        <v>843</v>
+      </c>
+      <c r="E731" s="8"/>
+    </row>
+    <row r="734" spans="1:5">
+      <c r="A734" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B734" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="C734" s="5"/>
+      <c r="D734" s="5"/>
+      <c r="E734" s="5"/>
     </row>
     <row r="735" spans="1:5">
       <c r="A735" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B735" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C735" s="6"/>
+      <c r="D735" s="6"/>
+      <c r="E735" s="6"/>
+    </row>
+    <row r="736" spans="1:5">
+      <c r="B736" s="8">
+        <v>0</v>
+      </c>
+      <c r="C736" s="8"/>
+      <c r="D736" s="8" t="s">
+        <v>844</v>
+      </c>
+      <c r="E736" s="8"/>
+    </row>
+    <row r="739" spans="1:5">
+      <c r="A739" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B735" s="5" t="s">
-        <v>850</v>
-      </c>
-      <c r="C735" s="5"/>
-      <c r="D735" s="5"/>
-      <c r="E735" s="5"/>
-    </row>
-    <row r="736" spans="1:5">
-      <c r="A736" s="4" t="s">
+      <c r="B739" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C739" s="5"/>
+      <c r="D739" s="5"/>
+      <c r="E739" s="5"/>
+    </row>
+    <row r="740" spans="1:5">
+      <c r="A740" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B736" s="6" t="s">
+      <c r="B740" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C740" s="6"/>
+      <c r="D740" s="6"/>
+      <c r="E740" s="6"/>
+    </row>
+    <row r="741" spans="1:5">
+      <c r="A741" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B741" s="6" t="s">
+        <v>840</v>
+      </c>
+      <c r="C741" s="6"/>
+      <c r="D741" s="6"/>
+      <c r="E741" s="6"/>
+    </row>
+    <row r="743" spans="1:5">
+      <c r="B743" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C743" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D743" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E743" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="744" spans="1:5">
+      <c r="B744" s="8">
+        <v>1</v>
+      </c>
+      <c r="C744" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="D744" s="8" t="s">
+        <v>860</v>
+      </c>
+      <c r="E744" s="8" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="745" spans="1:5">
+      <c r="B745" s="8">
+        <v>2</v>
+      </c>
+      <c r="C745" s="8" t="s">
+        <v>862</v>
+      </c>
+      <c r="D745" s="8" t="s">
+        <v>863</v>
+      </c>
+      <c r="E745" s="8" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="748" spans="1:5">
+      <c r="A748" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B748" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="C748" s="5"/>
+      <c r="D748" s="5"/>
+      <c r="E748" s="5"/>
+    </row>
+    <row r="749" spans="1:5">
+      <c r="A749" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B749" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C736" s="6"/>
-      <c r="D736" s="6"/>
-      <c r="E736" s="6"/>
-    </row>
-    <row r="737" spans="1:5">
-      <c r="A737" s="4" t="s">
+      <c r="C749" s="6"/>
+      <c r="D749" s="6"/>
+      <c r="E749" s="6"/>
+    </row>
+    <row r="750" spans="1:5">
+      <c r="A750" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B737" s="6" t="s">
-        <v>842</v>
-      </c>
-      <c r="C737" s="6"/>
-      <c r="D737" s="6"/>
-      <c r="E737" s="6"/>
-    </row>
-    <row r="739" spans="1:5">
-      <c r="B739" s="7" t="s">
+      <c r="B750" s="6" t="s">
+        <v>866</v>
+      </c>
+      <c r="C750" s="6"/>
+      <c r="D750" s="6"/>
+      <c r="E750" s="6"/>
+    </row>
+    <row r="752" spans="1:5">
+      <c r="B752" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C739" s="7" t="s">
+      <c r="C752" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D739" s="7" t="s">
+      <c r="D752" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E739" s="7" t="s">
+      <c r="E752" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="740" spans="1:5">
-      <c r="B740" s="8">
+    <row r="753" spans="1:5">
+      <c r="B753" s="8">
         <v>1</v>
       </c>
-      <c r="C740" s="8" t="s">
-        <v>851</v>
-      </c>
-      <c r="D740" s="8" t="s">
+      <c r="C753" s="8" t="s">
+        <v>867</v>
+      </c>
+      <c r="D753" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="E753" s="8" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="754" spans="1:5">
+      <c r="B754" s="8">
+        <v>2</v>
+      </c>
+      <c r="C754" s="8" t="s">
+        <v>869</v>
+      </c>
+      <c r="D754" s="8" t="s">
+        <v>588</v>
+      </c>
+      <c r="E754" s="8" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="755" spans="1:5">
+      <c r="B755" s="8">
+        <v>3</v>
+      </c>
+      <c r="C755" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="D755" s="8" t="s">
+        <v>872</v>
+      </c>
+      <c r="E755" s="8" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="758" spans="1:5">
+      <c r="A758" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B758" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="C758" s="5"/>
+      <c r="D758" s="5"/>
+      <c r="E758" s="5"/>
+    </row>
+    <row r="759" spans="1:5">
+      <c r="A759" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B759" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C759" s="6"/>
+      <c r="D759" s="6"/>
+      <c r="E759" s="6"/>
+    </row>
+    <row r="760" spans="1:5">
+      <c r="A760" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B760" s="6" t="s">
+        <v>866</v>
+      </c>
+      <c r="C760" s="6"/>
+      <c r="D760" s="6"/>
+      <c r="E760" s="6"/>
+    </row>
+    <row r="762" spans="1:5">
+      <c r="B762" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C762" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D762" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E762" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="763" spans="1:5">
+      <c r="B763" s="8">
+        <v>1</v>
+      </c>
+      <c r="C763" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="D763" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E740" s="8" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="743" spans="1:5">
-      <c r="A743" s="4" t="s">
+      <c r="E763" s="8" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="766" spans="1:5">
+      <c r="A766" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B743" s="5" t="s">
-        <v>853</v>
-      </c>
-      <c r="C743" s="5"/>
-      <c r="D743" s="5"/>
-      <c r="E743" s="5"/>
-    </row>
-    <row r="744" spans="1:5">
-      <c r="A744" s="4" t="s">
+      <c r="B766" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="C766" s="5"/>
+      <c r="D766" s="5"/>
+      <c r="E766" s="5"/>
+    </row>
+    <row r="767" spans="1:5">
+      <c r="A767" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B744" s="6" t="s">
+      <c r="B767" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C744" s="6"/>
-      <c r="D744" s="6"/>
-      <c r="E744" s="6"/>
-    </row>
-    <row r="745" spans="1:5">
-      <c r="A745" s="4" t="s">
+      <c r="C767" s="6"/>
+      <c r="D767" s="6"/>
+      <c r="E767" s="6"/>
+    </row>
+    <row r="768" spans="1:5">
+      <c r="A768" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B745" s="6" t="s">
-        <v>854</v>
-      </c>
-      <c r="C745" s="6"/>
-      <c r="D745" s="6"/>
-      <c r="E745" s="6"/>
+      <c r="B768" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="C768" s="6"/>
+      <c r="D768" s="6"/>
+      <c r="E768" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="198">
+  <mergeCells count="202">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B11:E11"/>
@@ -9884,35 +10192,39 @@
     <mergeCell ref="B652:E652"/>
     <mergeCell ref="B653:E653"/>
     <mergeCell ref="B654:E654"/>
-    <mergeCell ref="B661:E661"/>
-    <mergeCell ref="B662:E662"/>
-    <mergeCell ref="B663:E663"/>
-    <mergeCell ref="B674:E674"/>
-    <mergeCell ref="B675:E675"/>
-    <mergeCell ref="B683:E683"/>
+    <mergeCell ref="B672:E672"/>
+    <mergeCell ref="B673:E673"/>
+    <mergeCell ref="B677:E677"/>
+    <mergeCell ref="B678:E678"/>
     <mergeCell ref="B684:E684"/>
-    <mergeCell ref="B688:E688"/>
-    <mergeCell ref="B689:E689"/>
-    <mergeCell ref="B690:E690"/>
+    <mergeCell ref="B685:E685"/>
+    <mergeCell ref="B686:E686"/>
     <mergeCell ref="B697:E697"/>
     <mergeCell ref="B698:E698"/>
-    <mergeCell ref="B699:E699"/>
     <mergeCell ref="B706:E706"/>
     <mergeCell ref="B707:E707"/>
     <mergeCell ref="B711:E711"/>
     <mergeCell ref="B712:E712"/>
-    <mergeCell ref="B716:E716"/>
-    <mergeCell ref="B717:E717"/>
-    <mergeCell ref="B718:E718"/>
-    <mergeCell ref="B725:E725"/>
-    <mergeCell ref="B726:E726"/>
-    <mergeCell ref="B727:E727"/>
+    <mergeCell ref="B713:E713"/>
+    <mergeCell ref="B720:E720"/>
+    <mergeCell ref="B721:E721"/>
+    <mergeCell ref="B722:E722"/>
+    <mergeCell ref="B729:E729"/>
+    <mergeCell ref="B730:E730"/>
+    <mergeCell ref="B734:E734"/>
     <mergeCell ref="B735:E735"/>
-    <mergeCell ref="B736:E736"/>
-    <mergeCell ref="B737:E737"/>
-    <mergeCell ref="B743:E743"/>
-    <mergeCell ref="B744:E744"/>
-    <mergeCell ref="B745:E745"/>
+    <mergeCell ref="B739:E739"/>
+    <mergeCell ref="B740:E740"/>
+    <mergeCell ref="B741:E741"/>
+    <mergeCell ref="B748:E748"/>
+    <mergeCell ref="B749:E749"/>
+    <mergeCell ref="B750:E750"/>
+    <mergeCell ref="B758:E758"/>
+    <mergeCell ref="B759:E759"/>
+    <mergeCell ref="B760:E760"/>
+    <mergeCell ref="B766:E766"/>
+    <mergeCell ref="B767:E767"/>
+    <mergeCell ref="B768:E768"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11586,7 +11898,7 @@
         <v>56</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>822</v>
+        <v>846</v>
       </c>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -11596,7 +11908,7 @@
         <v>126</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>813</v>
+        <v>837</v>
       </c>
       <c r="C191" s="6"/>
       <c r="D191" s="6"/>
@@ -11617,10 +11929,10 @@
         <v>1</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>823</v>
+        <v>847</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>824</v>
+        <v>848</v>
       </c>
     </row>
     <row r="195" spans="2:4">
@@ -11628,10 +11940,10 @@
         <v>2</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>825</v>
+        <v>849</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>826</v>
+        <v>850</v>
       </c>
     </row>
     <row r="196" spans="2:4">
@@ -11639,10 +11951,10 @@
         <v>3</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>827</v>
+        <v>851</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>828</v>
+        <v>852</v>
       </c>
     </row>
     <row r="197" spans="2:4">
@@ -11650,10 +11962,10 @@
         <v>4</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>829</v>
+        <v>853</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>830</v>
+        <v>854</v>
       </c>
     </row>
     <row r="198" spans="2:4">
@@ -11661,10 +11973,10 @@
         <v>5</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>831</v>
+        <v>855</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>832</v>
+        <v>856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>